<commit_message>
1117 signup&login 기능 추가
</commit_message>
<xml_diff>
--- a/etc/연도별 박스오피스 순위.xlsx
+++ b/etc/연도별 박스오피스 순위.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimcalm/Desktop/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimcalm/Desktop/final-project/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2C7683-D659-C448-950D-1B3199DB103E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1E14D9-E603-844E-AEDC-201D06881528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1420" yWindow="500" windowWidth="36980" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4948" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4947" uniqueCount="1305">
   <si>
     <t>■ 연도별 박스오피스</t>
   </si>
@@ -4319,6 +4319,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4330,12 +4336,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -4620,8 +4620,8 @@
   <dimension ref="A1:X500"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A486" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <pane ySplit="6" topLeftCell="A342" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B361" sqref="B361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1"/>
@@ -4650,76 +4650,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18" customHeight="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
     </row>
     <row r="2" spans="1:24" ht="18" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" spans="1:24" ht="18" customHeight="1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
     </row>
     <row r="4" spans="1:24" ht="18" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1">
       <c r="A5" s="22">
@@ -5515,8 +5515,8 @@
       <c r="O17" s="28">
         <v>20040695</v>
       </c>
-      <c r="P17" s="17" t="s">
-        <v>64</v>
+      <c r="P17" s="28">
+        <v>20040695</v>
       </c>
       <c r="Q17" s="17" t="s">
         <v>65</v>
@@ -34522,8 +34522,8 @@
   <dimension ref="A1:G490"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C326" sqref="C326"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -34587,7 +34587,7 @@
       <c r="A3" s="38" t="s">
         <v>1302</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="42">
         <v>2007</v>
       </c>
       <c r="C3" s="39">
@@ -34610,7 +34610,7 @@
       <c r="A4" s="38" t="s">
         <v>1108</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="42">
         <v>2021</v>
       </c>
       <c r="C4" s="39">
@@ -34633,7 +34633,7 @@
       <c r="A5" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="42">
         <v>2006</v>
       </c>
       <c r="C5" s="39">
@@ -34656,7 +34656,7 @@
       <c r="A6" s="38" t="s">
         <v>416</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="42">
         <v>2012</v>
       </c>
       <c r="C6" s="39">
@@ -34679,7 +34679,7 @@
       <c r="A7" s="38" t="s">
         <v>1248</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="42">
         <v>2022</v>
       </c>
       <c r="C7" s="39">
@@ -34702,7 +34702,7 @@
       <c r="A8" s="38" t="s">
         <v>503</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="42">
         <v>2010</v>
       </c>
       <c r="C8" s="39">
@@ -34725,7 +34725,7 @@
       <c r="A9" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="42">
         <v>2005</v>
       </c>
       <c r="C9" s="39">
@@ -34748,7 +34748,7 @@
       <c r="A10" s="38" t="s">
         <v>1281</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="42">
         <v>2009</v>
       </c>
       <c r="C10" s="39">
@@ -34771,7 +34771,7 @@
       <c r="A11" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="42">
         <v>2007</v>
       </c>
       <c r="C11" s="39">
@@ -34794,7 +34794,7 @@
       <c r="A12" s="38" t="s">
         <v>407</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="42">
         <v>2008</v>
       </c>
       <c r="C12" s="39">
@@ -34817,7 +34817,7 @@
       <c r="A13" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="43">
         <v>2004</v>
       </c>
       <c r="C13" s="37">
@@ -34840,7 +34840,7 @@
       <c r="A14" s="38" t="s">
         <v>1186</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="42">
         <v>2021</v>
       </c>
       <c r="C14" s="39">
@@ -34863,7 +34863,7 @@
       <c r="A15" s="38" t="s">
         <v>946</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="42">
         <v>2017</v>
       </c>
       <c r="C15" s="39">
@@ -34886,7 +34886,7 @@
       <c r="A16" s="38" t="s">
         <v>804</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="42">
         <v>2016</v>
       </c>
       <c r="C16" s="39">
@@ -34909,7 +34909,7 @@
       <c r="A17" s="38" t="s">
         <v>732</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="42">
         <v>2013</v>
       </c>
       <c r="C17" s="39">
@@ -34932,7 +34932,7 @@
       <c r="A18" s="38" t="s">
         <v>840</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B18" s="42">
         <v>2019</v>
       </c>
       <c r="C18" s="39">
@@ -34955,7 +34955,7 @@
       <c r="A19" s="38" t="s">
         <v>1207</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="42">
         <v>2022</v>
       </c>
       <c r="C19" s="39">
@@ -34978,7 +34978,7 @@
       <c r="A20" s="38" t="s">
         <v>1095</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="42">
         <v>2019</v>
       </c>
       <c r="C20" s="39">
@@ -35001,7 +35001,7 @@
       <c r="A21" s="38" t="s">
         <v>603</v>
       </c>
-      <c r="B21" s="47">
+      <c r="B21" s="42">
         <v>2012</v>
       </c>
       <c r="C21" s="39">
@@ -35024,7 +35024,7 @@
       <c r="A22" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22" s="42">
         <v>2005</v>
       </c>
       <c r="C22" s="39">
@@ -35047,7 +35047,7 @@
       <c r="A23" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="B23" s="47">
+      <c r="B23" s="42">
         <v>2006</v>
       </c>
       <c r="C23" s="39">
@@ -35070,7 +35070,7 @@
       <c r="A24" s="38" t="s">
         <v>1093</v>
       </c>
-      <c r="B24" s="47">
+      <c r="B24" s="42">
         <v>2018</v>
       </c>
       <c r="C24" s="39">
@@ -35093,7 +35093,7 @@
       <c r="A25" s="38" t="s">
         <v>868</v>
       </c>
-      <c r="B25" s="47">
+      <c r="B25" s="42">
         <v>2017</v>
       </c>
       <c r="C25" s="39">
@@ -35116,7 +35116,7 @@
       <c r="A26" s="38" t="s">
         <v>1032</v>
       </c>
-      <c r="B26" s="47">
+      <c r="B26" s="42">
         <v>2017</v>
       </c>
       <c r="C26" s="39">
@@ -35139,7 +35139,7 @@
       <c r="A27" s="38" t="s">
         <v>443</v>
       </c>
-      <c r="B27" s="47">
+      <c r="B27" s="42">
         <v>2009</v>
       </c>
       <c r="C27" s="39">
@@ -35162,7 +35162,7 @@
       <c r="A28" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="B28" s="47">
+      <c r="B28" s="42">
         <v>2005</v>
       </c>
       <c r="C28" s="39">
@@ -35185,7 +35185,7 @@
       <c r="A29" s="38" t="s">
         <v>1045</v>
       </c>
-      <c r="B29" s="47">
+      <c r="B29" s="42">
         <v>2018</v>
       </c>
       <c r="C29" s="39">
@@ -35208,7 +35208,7 @@
       <c r="A30" s="38" t="s">
         <v>1043</v>
       </c>
-      <c r="B30" s="47">
+      <c r="B30" s="42">
         <v>2018</v>
       </c>
       <c r="C30" s="39">
@@ -35231,7 +35231,7 @@
       <c r="A31" s="38" t="s">
         <v>662</v>
       </c>
-      <c r="B31" s="47">
+      <c r="B31" s="42">
         <v>2012</v>
       </c>
       <c r="C31" s="39">
@@ -35254,7 +35254,7 @@
       <c r="A32" s="38" t="s">
         <v>650</v>
       </c>
-      <c r="B32" s="47">
+      <c r="B32" s="42">
         <v>2012</v>
       </c>
       <c r="C32" s="39">
@@ -35277,7 +35277,7 @@
       <c r="A33" s="38" t="s">
         <v>1119</v>
       </c>
-      <c r="B33" s="47">
+      <c r="B33" s="42">
         <v>2019</v>
       </c>
       <c r="C33" s="39">
@@ -35300,7 +35300,7 @@
       <c r="A34" s="38" t="s">
         <v>762</v>
       </c>
-      <c r="B34" s="47">
+      <c r="B34" s="42">
         <v>2016</v>
       </c>
       <c r="C34" s="39">
@@ -35323,7 +35323,7 @@
       <c r="A35" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="B35" s="47">
+      <c r="B35" s="42">
         <v>2007</v>
       </c>
       <c r="C35" s="39">
@@ -35346,7 +35346,7 @@
       <c r="A36" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="B36" s="47">
+      <c r="B36" s="42">
         <v>2009</v>
       </c>
       <c r="C36" s="39">
@@ -35369,7 +35369,7 @@
       <c r="A37" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="B37" s="47">
+      <c r="B37" s="42">
         <v>2019</v>
       </c>
       <c r="C37" s="39">
@@ -35392,7 +35392,7 @@
       <c r="A38" s="38" t="s">
         <v>1019</v>
       </c>
-      <c r="B38" s="47">
+      <c r="B38" s="42">
         <v>2018</v>
       </c>
       <c r="C38" s="39">
@@ -35415,7 +35415,7 @@
       <c r="A39" s="38" t="s">
         <v>1150</v>
       </c>
-      <c r="B39" s="47">
+      <c r="B39" s="42">
         <v>2020</v>
       </c>
       <c r="C39" s="39">
@@ -35438,7 +35438,7 @@
       <c r="A40" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="B40" s="47">
+      <c r="B40" s="42">
         <v>2006</v>
       </c>
       <c r="C40" s="39">
@@ -35461,7 +35461,7 @@
       <c r="A41" s="38" t="s">
         <v>888</v>
       </c>
-      <c r="B41" s="47">
+      <c r="B41" s="42">
         <v>2016</v>
       </c>
       <c r="C41" s="39">
@@ -35484,7 +35484,7 @@
       <c r="A42" s="38" t="s">
         <v>540</v>
       </c>
-      <c r="B42" s="47">
+      <c r="B42" s="42">
         <v>2011</v>
       </c>
       <c r="C42" s="39">
@@ -35507,7 +35507,7 @@
       <c r="A43" s="38" t="s">
         <v>576</v>
       </c>
-      <c r="B43" s="47">
+      <c r="B43" s="42">
         <v>2012</v>
       </c>
       <c r="C43" s="39">
@@ -35530,7 +35530,7 @@
       <c r="A44" s="38" t="s">
         <v>987</v>
       </c>
-      <c r="B44" s="47">
+      <c r="B44" s="42">
         <v>2018</v>
       </c>
       <c r="C44" s="39">
@@ -35553,7 +35553,7 @@
       <c r="A45" s="38" t="s">
         <v>1053</v>
       </c>
-      <c r="B45" s="47">
+      <c r="B45" s="42">
         <v>2020</v>
       </c>
       <c r="C45" s="39">
@@ -35576,7 +35576,7 @@
       <c r="A46" s="38" t="s">
         <v>729</v>
       </c>
-      <c r="B46" s="47">
+      <c r="B46" s="42">
         <v>2017</v>
       </c>
       <c r="C46" s="39">
@@ -35599,7 +35599,7 @@
       <c r="A47" s="38" t="s">
         <v>847</v>
       </c>
-      <c r="B47" s="47">
+      <c r="B47" s="42">
         <v>2014</v>
       </c>
       <c r="C47" s="39">
@@ -35622,7 +35622,7 @@
       <c r="A48" s="38" t="s">
         <v>852</v>
       </c>
-      <c r="B48" s="47">
+      <c r="B48" s="42">
         <v>2015</v>
       </c>
       <c r="C48" s="39">
@@ -35645,7 +35645,7 @@
       <c r="A49" s="38" t="s">
         <v>1279</v>
       </c>
-      <c r="B49" s="47">
+      <c r="B49" s="42">
         <v>2022</v>
       </c>
       <c r="C49" s="39">
@@ -35668,7 +35668,7 @@
       <c r="A50" s="38" t="s">
         <v>985</v>
       </c>
-      <c r="B50" s="47">
+      <c r="B50" s="42">
         <v>2018</v>
       </c>
       <c r="C50" s="39">
@@ -35691,7 +35691,7 @@
       <c r="A51" s="38" t="s">
         <v>1275</v>
       </c>
-      <c r="B51" s="47">
+      <c r="B51" s="42">
         <v>2022</v>
       </c>
       <c r="C51" s="39">
@@ -35714,7 +35714,7 @@
       <c r="A52" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B52" s="47">
+      <c r="B52" s="42">
         <v>2005</v>
       </c>
       <c r="C52" s="39">
@@ -35737,7 +35737,7 @@
       <c r="A53" s="38" t="s">
         <v>1089</v>
       </c>
-      <c r="B53" s="47">
+      <c r="B53" s="42">
         <v>2018</v>
       </c>
       <c r="C53" s="39">
@@ -35760,7 +35760,7 @@
       <c r="A54" s="38" t="s">
         <v>1262</v>
       </c>
-      <c r="B54" s="47">
+      <c r="B54" s="42">
         <v>2021</v>
       </c>
       <c r="C54" s="39">
@@ -35783,7 +35783,7 @@
       <c r="A55" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B55" s="48">
+      <c r="B55" s="43">
         <v>2004</v>
       </c>
       <c r="C55" s="37">
@@ -35806,7 +35806,7 @@
       <c r="A56" s="38" t="s">
         <v>927</v>
       </c>
-      <c r="B56" s="47">
+      <c r="B56" s="42">
         <v>2016</v>
       </c>
       <c r="C56" s="39">
@@ -35829,7 +35829,7 @@
       <c r="A57" s="38" t="s">
         <v>813</v>
       </c>
-      <c r="B57" s="47">
+      <c r="B57" s="42">
         <v>2014</v>
       </c>
       <c r="C57" s="39">
@@ -35852,7 +35852,7 @@
       <c r="A58" s="38" t="s">
         <v>1060</v>
       </c>
-      <c r="B58" s="47">
+      <c r="B58" s="42">
         <v>2019</v>
       </c>
       <c r="C58" s="39">
@@ -35875,7 +35875,7 @@
       <c r="A59" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="B59" s="47">
+      <c r="B59" s="42">
         <v>2005</v>
       </c>
       <c r="C59" s="39">
@@ -35898,7 +35898,7 @@
       <c r="A60" s="38" t="s">
         <v>434</v>
       </c>
-      <c r="B60" s="47">
+      <c r="B60" s="42">
         <v>2009</v>
       </c>
       <c r="C60" s="39">
@@ -35921,7 +35921,7 @@
       <c r="A61" s="38" t="s">
         <v>617</v>
       </c>
-      <c r="B61" s="47">
+      <c r="B61" s="42">
         <v>2011</v>
       </c>
       <c r="C61" s="39">
@@ -35944,7 +35944,7 @@
       <c r="A62" s="38" t="s">
         <v>424</v>
       </c>
-      <c r="B62" s="47">
+      <c r="B62" s="42">
         <v>2009</v>
       </c>
       <c r="C62" s="39">
@@ -35967,7 +35967,7 @@
       <c r="A63" s="38" t="s">
         <v>490</v>
       </c>
-      <c r="B63" s="47">
+      <c r="B63" s="42">
         <v>2010</v>
       </c>
       <c r="C63" s="39">
@@ -35990,7 +35990,7 @@
       <c r="A64" s="38" t="s">
         <v>462</v>
       </c>
-      <c r="B64" s="47">
+      <c r="B64" s="42">
         <v>2009</v>
       </c>
       <c r="C64" s="39">
@@ -36013,7 +36013,7 @@
       <c r="A65" s="38" t="s">
         <v>838</v>
       </c>
-      <c r="B65" s="47">
+      <c r="B65" s="42">
         <v>2020</v>
       </c>
       <c r="C65" s="39">
@@ -36036,7 +36036,7 @@
       <c r="A66" s="38" t="s">
         <v>636</v>
       </c>
-      <c r="B66" s="47">
+      <c r="B66" s="42">
         <v>2013</v>
       </c>
       <c r="C66" s="39">
@@ -36059,7 +36059,7 @@
       <c r="A67" s="38" t="s">
         <v>1116</v>
       </c>
-      <c r="B67" s="47">
+      <c r="B67" s="42">
         <v>2020</v>
       </c>
       <c r="C67" s="39">
@@ -36082,7 +36082,7 @@
       <c r="A68" s="38" t="s">
         <v>876</v>
       </c>
-      <c r="B68" s="47">
+      <c r="B68" s="42">
         <v>2016</v>
       </c>
       <c r="C68" s="39">
@@ -36105,7 +36105,7 @@
       <c r="A69" s="38" t="s">
         <v>664</v>
       </c>
-      <c r="B69" s="47">
+      <c r="B69" s="42">
         <v>2012</v>
       </c>
       <c r="C69" s="39">
@@ -36128,7 +36128,7 @@
       <c r="A70" s="38" t="s">
         <v>879</v>
       </c>
-      <c r="B70" s="47">
+      <c r="B70" s="42">
         <v>2017</v>
       </c>
       <c r="C70" s="39">
@@ -36151,7 +36151,7 @@
       <c r="A71" s="38" t="s">
         <v>1237</v>
       </c>
-      <c r="B71" s="47">
+      <c r="B71" s="42">
         <v>2022</v>
       </c>
       <c r="C71" s="39">
@@ -36174,7 +36174,7 @@
       <c r="A72" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="47">
+      <c r="B72" s="42">
         <v>2005</v>
       </c>
       <c r="C72" s="39">
@@ -36197,7 +36197,7 @@
       <c r="A73" s="38" t="s">
         <v>1277</v>
       </c>
-      <c r="B73" s="47">
+      <c r="B73" s="42">
         <v>2022</v>
       </c>
       <c r="C73" s="39">
@@ -36220,7 +36220,7 @@
       <c r="A74" s="38" t="s">
         <v>1138</v>
       </c>
-      <c r="B74" s="47">
+      <c r="B74" s="42">
         <v>2019</v>
       </c>
       <c r="C74" s="39">
@@ -36243,7 +36243,7 @@
       <c r="A75" s="38" t="s">
         <v>1241</v>
       </c>
-      <c r="B75" s="47">
+      <c r="B75" s="42">
         <v>2021</v>
       </c>
       <c r="C75" s="39">
@@ -36266,7 +36266,7 @@
       <c r="A76" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="B76" s="47">
+      <c r="B76" s="42">
         <v>2005</v>
       </c>
       <c r="C76" s="39">
@@ -36289,7 +36289,7 @@
       <c r="A77" s="38" t="s">
         <v>521</v>
       </c>
-      <c r="B77" s="47">
+      <c r="B77" s="42">
         <v>2010</v>
       </c>
       <c r="C77" s="39">
@@ -36312,7 +36312,7 @@
       <c r="A78" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B78" s="47">
+      <c r="B78" s="42">
         <v>2005</v>
       </c>
       <c r="C78" s="39">
@@ -36335,7 +36335,7 @@
       <c r="A79" s="38" t="s">
         <v>607</v>
       </c>
-      <c r="B79" s="47">
+      <c r="B79" s="42">
         <v>2012</v>
       </c>
       <c r="C79" s="39">
@@ -36358,7 +36358,7 @@
       <c r="A80" s="38" t="s">
         <v>1038</v>
       </c>
-      <c r="B80" s="47">
+      <c r="B80" s="42">
         <v>2018</v>
       </c>
       <c r="C80" s="39">
@@ -36381,7 +36381,7 @@
       <c r="A81" s="38" t="s">
         <v>924</v>
       </c>
-      <c r="B81" s="47">
+      <c r="B81" s="42">
         <v>2012</v>
       </c>
       <c r="C81" s="39">
@@ -36404,7 +36404,7 @@
       <c r="A82" s="38" t="s">
         <v>831</v>
       </c>
-      <c r="B82" s="47">
+      <c r="B82" s="42">
         <v>2014</v>
       </c>
       <c r="C82" s="39">
@@ -36427,7 +36427,7 @@
       <c r="A83" s="38" t="s">
         <v>892</v>
       </c>
-      <c r="B83" s="47">
+      <c r="B83" s="42">
         <v>2016</v>
       </c>
       <c r="C83" s="39">
@@ -36450,7 +36450,7 @@
       <c r="A84" s="38" t="s">
         <v>1016</v>
       </c>
-      <c r="B84" s="47">
+      <c r="B84" s="42">
         <v>2018</v>
       </c>
       <c r="C84" s="39">
@@ -36473,7 +36473,7 @@
       <c r="A85" s="38" t="s">
         <v>385</v>
       </c>
-      <c r="B85" s="47">
+      <c r="B85" s="42">
         <v>2008</v>
       </c>
       <c r="C85" s="39">
@@ -36496,7 +36496,7 @@
       <c r="A86" s="38" t="s">
         <v>1214</v>
       </c>
-      <c r="B86" s="47">
+      <c r="B86" s="42">
         <v>2022</v>
       </c>
       <c r="C86" s="39">
@@ -36519,7 +36519,7 @@
       <c r="A87" s="38" t="s">
         <v>1025</v>
       </c>
-      <c r="B87" s="47">
+      <c r="B87" s="42">
         <v>2018</v>
       </c>
       <c r="C87" s="39">
@@ -36542,7 +36542,7 @@
       <c r="A88" s="38" t="s">
         <v>1158</v>
       </c>
-      <c r="B88" s="47">
+      <c r="B88" s="42">
         <v>2020</v>
       </c>
       <c r="C88" s="39">
@@ -36565,7 +36565,7 @@
       <c r="A89" s="38" t="s">
         <v>1173</v>
       </c>
-      <c r="B89" s="47">
+      <c r="B89" s="42">
         <v>2021</v>
       </c>
       <c r="C89" s="39">
@@ -36588,7 +36588,7 @@
       <c r="A90" s="38" t="s">
         <v>656</v>
       </c>
-      <c r="B90" s="47">
+      <c r="B90" s="42">
         <v>2012</v>
       </c>
       <c r="C90" s="39">
@@ -36611,7 +36611,7 @@
       <c r="A91" s="38" t="s">
         <v>994</v>
       </c>
-      <c r="B91" s="47">
+      <c r="B91" s="42">
         <v>2017</v>
       </c>
       <c r="C91" s="39">
@@ -36634,7 +36634,7 @@
       <c r="A92" s="38" t="s">
         <v>844</v>
       </c>
-      <c r="B92" s="47">
+      <c r="B92" s="42">
         <v>2015</v>
       </c>
       <c r="C92" s="39">
@@ -36657,7 +36657,7 @@
       <c r="A93" s="38" t="s">
         <v>538</v>
       </c>
-      <c r="B93" s="47">
+      <c r="B93" s="42">
         <v>2011</v>
       </c>
       <c r="C93" s="39">
@@ -36680,7 +36680,7 @@
       <c r="A94" s="38" t="s">
         <v>1040</v>
       </c>
-      <c r="B94" s="47">
+      <c r="B94" s="42">
         <v>2018</v>
       </c>
       <c r="C94" s="39">
@@ -36703,7 +36703,7 @@
       <c r="A95" s="38" t="s">
         <v>873</v>
       </c>
-      <c r="B95" s="47">
+      <c r="B95" s="42">
         <v>2020</v>
       </c>
       <c r="C95" s="39">
@@ -36726,7 +36726,7 @@
       <c r="A96" s="38" t="s">
         <v>950</v>
       </c>
-      <c r="B96" s="47">
+      <c r="B96" s="42">
         <v>2016</v>
       </c>
       <c r="C96" s="39">
@@ -36749,7 +36749,7 @@
       <c r="A97" s="38" t="s">
         <v>1231</v>
       </c>
-      <c r="B97" s="47">
+      <c r="B97" s="42">
         <v>2022</v>
       </c>
       <c r="C97" s="39">
@@ -36772,7 +36772,7 @@
       <c r="A98" s="38" t="s">
         <v>1219</v>
       </c>
-      <c r="B98" s="47">
+      <c r="B98" s="42">
         <v>2021</v>
       </c>
       <c r="C98" s="39">
@@ -36795,7 +36795,7 @@
       <c r="A99" s="38" t="s">
         <v>959</v>
       </c>
-      <c r="B99" s="47">
+      <c r="B99" s="42">
         <v>2017</v>
       </c>
       <c r="C99" s="39">
@@ -36818,7 +36818,7 @@
       <c r="A100" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B100" s="47">
+      <c r="B100" s="42">
         <v>2007</v>
       </c>
       <c r="C100" s="39">
@@ -36841,7 +36841,7 @@
       <c r="A101" s="38" t="s">
         <v>395</v>
       </c>
-      <c r="B101" s="47">
+      <c r="B101" s="42">
         <v>2008</v>
       </c>
       <c r="C101" s="39">
@@ -36864,7 +36864,7 @@
       <c r="A102" s="38" t="s">
         <v>825</v>
       </c>
-      <c r="B102" s="47">
+      <c r="B102" s="42">
         <v>2014</v>
       </c>
       <c r="C102" s="39">
@@ -36887,7 +36887,7 @@
       <c r="A103" s="38" t="s">
         <v>1148</v>
       </c>
-      <c r="B103" s="47">
+      <c r="B103" s="42">
         <v>2022</v>
       </c>
       <c r="C103" s="39">
@@ -36910,7 +36910,7 @@
       <c r="A104" s="38" t="s">
         <v>914</v>
       </c>
-      <c r="B104" s="47">
+      <c r="B104" s="42">
         <v>2014</v>
       </c>
       <c r="C104" s="39">
@@ -36933,7 +36933,7 @@
       <c r="A105" s="38" t="s">
         <v>1221</v>
       </c>
-      <c r="B105" s="47">
+      <c r="B105" s="42">
         <v>2021</v>
       </c>
       <c r="C105" s="39">
@@ -36956,7 +36956,7 @@
       <c r="A106" s="38" t="s">
         <v>1184</v>
       </c>
-      <c r="B106" s="47">
+      <c r="B106" s="42">
         <v>2021</v>
       </c>
       <c r="C106" s="39">
@@ -36979,7 +36979,7 @@
       <c r="A107" s="38" t="s">
         <v>1256</v>
       </c>
-      <c r="B107" s="47">
+      <c r="B107" s="42">
         <v>2021</v>
       </c>
       <c r="C107" s="39">
@@ -37002,7 +37002,7 @@
       <c r="A108" s="38" t="s">
         <v>1063</v>
       </c>
-      <c r="B108" s="47">
+      <c r="B108" s="42">
         <v>2019</v>
       </c>
       <c r="C108" s="39">
@@ -37025,7 +37025,7 @@
       <c r="A109" s="38" t="s">
         <v>370</v>
       </c>
-      <c r="B109" s="47">
+      <c r="B109" s="42">
         <v>2008</v>
       </c>
       <c r="C109" s="39">
@@ -37048,7 +37048,7 @@
       <c r="A110" s="38" t="s">
         <v>866</v>
       </c>
-      <c r="B110" s="47">
+      <c r="B110" s="42">
         <v>2017</v>
       </c>
       <c r="C110" s="39">
@@ -37071,7 +37071,7 @@
       <c r="A111" s="38" t="s">
         <v>939</v>
       </c>
-      <c r="B111" s="47">
+      <c r="B111" s="42">
         <v>2016</v>
       </c>
       <c r="C111" s="39">
@@ -37094,7 +37094,7 @@
       <c r="A112" s="38" t="s">
         <v>1013</v>
       </c>
-      <c r="B112" s="47">
+      <c r="B112" s="42">
         <v>2018</v>
       </c>
       <c r="C112" s="39">
@@ -37117,7 +37117,7 @@
       <c r="A113" s="38" t="s">
         <v>1229</v>
       </c>
-      <c r="B113" s="47">
+      <c r="B113" s="42">
         <v>2022</v>
       </c>
       <c r="C113" s="39">
@@ -37140,7 +37140,7 @@
       <c r="A114" s="38" t="s">
         <v>790</v>
       </c>
-      <c r="B114" s="47">
+      <c r="B114" s="42">
         <v>2015</v>
       </c>
       <c r="C114" s="39">
@@ -37163,7 +37163,7 @@
       <c r="A115" s="38" t="s">
         <v>1190</v>
       </c>
-      <c r="B115" s="47">
+      <c r="B115" s="42">
         <v>2021</v>
       </c>
       <c r="C115" s="39">
@@ -37186,7 +37186,7 @@
       <c r="A116" s="38" t="s">
         <v>1152</v>
       </c>
-      <c r="B116" s="47">
+      <c r="B116" s="42">
         <v>2019</v>
       </c>
       <c r="C116" s="39">
@@ -37209,7 +37209,7 @@
       <c r="A117" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="B117" s="48">
+      <c r="B117" s="43">
         <v>2004</v>
       </c>
       <c r="C117" s="37">
@@ -37232,7 +37232,7 @@
       <c r="A118" s="38" t="s">
         <v>921</v>
       </c>
-      <c r="B118" s="47">
+      <c r="B118" s="42">
         <v>2016</v>
       </c>
       <c r="C118" s="39">
@@ -37255,7 +37255,7 @@
       <c r="A119" s="38" t="s">
         <v>678</v>
       </c>
-      <c r="B119" s="47">
+      <c r="B119" s="42">
         <v>2013</v>
       </c>
       <c r="C119" s="39">
@@ -37278,7 +37278,7 @@
       <c r="A120" s="38" t="s">
         <v>1081</v>
       </c>
-      <c r="B120" s="47">
+      <c r="B120" s="42">
         <v>2019</v>
       </c>
       <c r="C120" s="39">
@@ -37301,7 +37301,7 @@
       <c r="A121" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="B121" s="47">
+      <c r="B121" s="42">
         <v>2006</v>
       </c>
       <c r="C121" s="39">
@@ -37324,7 +37324,7 @@
       <c r="A122" s="38" t="s">
         <v>718</v>
       </c>
-      <c r="B122" s="47">
+      <c r="B122" s="42">
         <v>2010</v>
       </c>
       <c r="C122" s="39">
@@ -37347,7 +37347,7 @@
       <c r="A123" s="38" t="s">
         <v>310</v>
       </c>
-      <c r="B123" s="47">
+      <c r="B123" s="42">
         <v>2008</v>
       </c>
       <c r="C123" s="39">
@@ -37370,7 +37370,7 @@
       <c r="A124" s="38" t="s">
         <v>744</v>
       </c>
-      <c r="B124" s="47">
+      <c r="B124" s="42">
         <v>2014</v>
       </c>
       <c r="C124" s="39">
@@ -37393,7 +37393,7 @@
       <c r="A125" s="38" t="s">
         <v>1156</v>
       </c>
-      <c r="B125" s="47">
+      <c r="B125" s="42">
         <v>2019</v>
       </c>
       <c r="C125" s="39">
@@ -37416,7 +37416,7 @@
       <c r="A126" s="38" t="s">
         <v>467</v>
       </c>
-      <c r="B126" s="47">
+      <c r="B126" s="42">
         <v>2009</v>
       </c>
       <c r="C126" s="39">
@@ -37439,7 +37439,7 @@
       <c r="A127" s="38" t="s">
         <v>747</v>
       </c>
-      <c r="B127" s="47">
+      <c r="B127" s="42">
         <v>2015</v>
       </c>
       <c r="C127" s="39">
@@ -37462,7 +37462,7 @@
       <c r="A128" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B128" s="48">
+      <c r="B128" s="43">
         <v>2004</v>
       </c>
       <c r="C128" s="37">
@@ -37485,7 +37485,7 @@
       <c r="A129" s="38" t="s">
         <v>543</v>
       </c>
-      <c r="B129" s="47">
+      <c r="B129" s="42">
         <v>2011</v>
       </c>
       <c r="C129" s="39">
@@ -37508,7 +37508,7 @@
       <c r="A130" s="38" t="s">
         <v>1239</v>
       </c>
-      <c r="B130" s="47">
+      <c r="B130" s="42">
         <v>2021</v>
       </c>
       <c r="C130" s="39">
@@ -37531,7 +37531,7 @@
       <c r="A131" s="38" t="s">
         <v>318</v>
       </c>
-      <c r="B131" s="47">
+      <c r="B131" s="42">
         <v>2007</v>
       </c>
       <c r="C131" s="39">
@@ -37554,7 +37554,7 @@
       <c r="A132" s="38" t="s">
         <v>1047</v>
       </c>
-      <c r="B132" s="47">
+      <c r="B132" s="42">
         <v>2018</v>
       </c>
       <c r="C132" s="39">
@@ -37577,7 +37577,7 @@
       <c r="A133" s="38" t="s">
         <v>472</v>
       </c>
-      <c r="B133" s="47">
+      <c r="B133" s="42">
         <v>2009</v>
       </c>
       <c r="C133" s="39">
@@ -37600,7 +37600,7 @@
       <c r="A134" s="38" t="s">
         <v>469</v>
       </c>
-      <c r="B134" s="47">
+      <c r="B134" s="42">
         <v>2009</v>
       </c>
       <c r="C134" s="39">
@@ -37623,7 +37623,7 @@
       <c r="A135" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="B135" s="47">
+      <c r="B135" s="42">
         <v>2013</v>
       </c>
       <c r="C135" s="39">
@@ -37646,7 +37646,7 @@
       <c r="A136" s="38" t="s">
         <v>952</v>
       </c>
-      <c r="B136" s="47">
+      <c r="B136" s="42">
         <v>2017</v>
       </c>
       <c r="C136" s="39">
@@ -37669,7 +37669,7 @@
       <c r="A137" s="38" t="s">
         <v>545</v>
       </c>
-      <c r="B137" s="47">
+      <c r="B137" s="42">
         <v>2011</v>
       </c>
       <c r="C137" s="39">
@@ -37692,7 +37692,7 @@
       <c r="A138" s="38" t="s">
         <v>437</v>
       </c>
-      <c r="B138" s="47">
+      <c r="B138" s="42">
         <v>2009</v>
       </c>
       <c r="C138" s="39">
@@ -37715,7 +37715,7 @@
       <c r="A139" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="B139" s="47">
+      <c r="B139" s="42">
         <v>2006</v>
       </c>
       <c r="C139" s="39">
@@ -37738,7 +37738,7 @@
       <c r="A140" s="38" t="s">
         <v>363</v>
       </c>
-      <c r="B140" s="47">
+      <c r="B140" s="42">
         <v>2008</v>
       </c>
       <c r="C140" s="39">
@@ -37761,7 +37761,7 @@
       <c r="A141" s="38" t="s">
         <v>1210</v>
       </c>
-      <c r="B141" s="47">
+      <c r="B141" s="42">
         <v>2022</v>
       </c>
       <c r="C141" s="39">
@@ -37784,7 +37784,7 @@
       <c r="A142" s="38" t="s">
         <v>1126</v>
       </c>
-      <c r="B142" s="47">
+      <c r="B142" s="42">
         <v>2021</v>
       </c>
       <c r="C142" s="39">
@@ -37807,7 +37807,7 @@
       <c r="A143" s="38" t="s">
         <v>1204</v>
       </c>
-      <c r="B143" s="47">
+      <c r="B143" s="42">
         <v>2010</v>
       </c>
       <c r="C143" s="39">
@@ -37830,7 +37830,7 @@
       <c r="A144" s="38" t="s">
         <v>573</v>
       </c>
-      <c r="B144" s="47">
+      <c r="B144" s="42">
         <v>2011</v>
       </c>
       <c r="C144" s="39">
@@ -37853,7 +37853,7 @@
       <c r="A145" s="38" t="s">
         <v>535</v>
       </c>
-      <c r="B145" s="47">
+      <c r="B145" s="42">
         <v>2010</v>
       </c>
       <c r="C145" s="39">
@@ -37876,7 +37876,7 @@
       <c r="A146" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="B146" s="47">
+      <c r="B146" s="42">
         <v>2005</v>
       </c>
       <c r="C146" s="39">
@@ -37899,7 +37899,7 @@
       <c r="A147" s="38" t="s">
         <v>464</v>
       </c>
-      <c r="B147" s="47">
+      <c r="B147" s="42">
         <v>2009</v>
       </c>
       <c r="C147" s="39">
@@ -37922,7 +37922,7 @@
       <c r="A148" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="B148" s="47">
+      <c r="B148" s="42">
         <v>2007</v>
       </c>
       <c r="C148" s="39">
@@ -37945,7 +37945,7 @@
       <c r="A149" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="B149" s="48">
+      <c r="B149" s="43">
         <v>2004</v>
       </c>
       <c r="C149" s="37">
@@ -37968,7 +37968,7 @@
       <c r="A150" s="38" t="s">
         <v>533</v>
       </c>
-      <c r="B150" s="47">
+      <c r="B150" s="42">
         <v>2010</v>
       </c>
       <c r="C150" s="39">
@@ -37991,7 +37991,7 @@
       <c r="A151" s="38" t="s">
         <v>652</v>
       </c>
-      <c r="B151" s="47">
+      <c r="B151" s="42">
         <v>2012</v>
       </c>
       <c r="C151" s="39">
@@ -38014,7 +38014,7 @@
       <c r="A152" s="38" t="s">
         <v>954</v>
       </c>
-      <c r="B152" s="47">
+      <c r="B152" s="42">
         <v>2013</v>
       </c>
       <c r="C152" s="39">
@@ -38037,7 +38037,7 @@
       <c r="A153" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="B153" s="47">
+      <c r="B153" s="42">
         <v>2007</v>
       </c>
       <c r="C153" s="39">
@@ -38060,7 +38060,7 @@
       <c r="A154" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="B154" s="47">
+      <c r="B154" s="42">
         <v>2007</v>
       </c>
       <c r="C154" s="39">
@@ -38083,7 +38083,7 @@
       <c r="A155" s="38" t="s">
         <v>1049</v>
       </c>
-      <c r="B155" s="47">
+      <c r="B155" s="42">
         <v>2019</v>
       </c>
       <c r="C155" s="39">
@@ -38106,7 +38106,7 @@
       <c r="A156" s="38" t="s">
         <v>1114</v>
       </c>
-      <c r="B156" s="47">
+      <c r="B156" s="42">
         <v>2020</v>
       </c>
       <c r="C156" s="39">
@@ -38129,7 +38129,7 @@
       <c r="A157" s="38" t="s">
         <v>1128</v>
       </c>
-      <c r="B157" s="47">
+      <c r="B157" s="42">
         <v>2020</v>
       </c>
       <c r="C157" s="39">
@@ -38152,7 +38152,7 @@
       <c r="A158" s="38" t="s">
         <v>1266</v>
       </c>
-      <c r="B158" s="47">
+      <c r="B158" s="42">
         <v>2022</v>
       </c>
       <c r="C158" s="39">
@@ -38175,7 +38175,7 @@
       <c r="A159" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="B159" s="47">
+      <c r="B159" s="42">
         <v>2021</v>
       </c>
       <c r="C159" s="39">
@@ -38198,7 +38198,7 @@
       <c r="A160" s="38" t="s">
         <v>492</v>
       </c>
-      <c r="B160" s="47">
+      <c r="B160" s="42">
         <v>2010</v>
       </c>
       <c r="C160" s="39">
@@ -38221,7 +38221,7 @@
       <c r="A161" s="38" t="s">
         <v>712</v>
       </c>
-      <c r="B161" s="47">
+      <c r="B161" s="42">
         <v>2014</v>
       </c>
       <c r="C161" s="39">
@@ -38244,7 +38244,7 @@
       <c r="A162" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="B162" s="48">
+      <c r="B162" s="43">
         <v>2004</v>
       </c>
       <c r="C162" s="37">
@@ -38267,7 +38267,7 @@
       <c r="A163" s="38" t="s">
         <v>1225</v>
       </c>
-      <c r="B163" s="47">
+      <c r="B163" s="42">
         <v>2022</v>
       </c>
       <c r="C163" s="39">
@@ -38290,7 +38290,7 @@
       <c r="A164" s="38" t="s">
         <v>642</v>
       </c>
-      <c r="B164" s="47">
+      <c r="B164" s="42">
         <v>2013</v>
       </c>
       <c r="C164" s="39">
@@ -38313,7 +38313,7 @@
       <c r="A165" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="B165" s="47">
+      <c r="B165" s="42">
         <v>2007</v>
       </c>
       <c r="C165" s="39">
@@ -38336,7 +38336,7 @@
       <c r="A166" s="38" t="s">
         <v>998</v>
       </c>
-      <c r="B166" s="47">
+      <c r="B166" s="42">
         <v>2017</v>
       </c>
       <c r="C166" s="39">
@@ -38359,7 +38359,7 @@
       <c r="A167" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="B167" s="48">
+      <c r="B167" s="43">
         <v>2004</v>
       </c>
       <c r="C167" s="37">
@@ -38382,7 +38382,7 @@
       <c r="A168" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B168" s="48">
+      <c r="B168" s="43">
         <v>2004</v>
       </c>
       <c r="C168" s="37">
@@ -38405,7 +38405,7 @@
       <c r="A169" s="38" t="s">
         <v>505</v>
       </c>
-      <c r="B169" s="47">
+      <c r="B169" s="42">
         <v>2010</v>
       </c>
       <c r="C169" s="39">
@@ -38428,7 +38428,7 @@
       <c r="A170" s="38" t="s">
         <v>1068</v>
       </c>
-      <c r="B170" s="47">
+      <c r="B170" s="42">
         <v>2018</v>
       </c>
       <c r="C170" s="39">
@@ -38451,7 +38451,7 @@
       <c r="A171" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="B171" s="47">
+      <c r="B171" s="42">
         <v>2008</v>
       </c>
       <c r="C171" s="39">
@@ -38474,7 +38474,7 @@
       <c r="A172" s="38" t="s">
         <v>857</v>
       </c>
-      <c r="B172" s="47">
+      <c r="B172" s="42">
         <v>2020</v>
       </c>
       <c r="C172" s="39">
@@ -38497,7 +38497,7 @@
       <c r="A173" s="38" t="s">
         <v>1091</v>
       </c>
-      <c r="B173" s="47">
+      <c r="B173" s="42">
         <v>2019</v>
       </c>
       <c r="C173" s="39">
@@ -38520,7 +38520,7 @@
       <c r="A174" s="38" t="s">
         <v>836</v>
       </c>
-      <c r="B174" s="47">
+      <c r="B174" s="42">
         <v>2015</v>
       </c>
       <c r="C174" s="39">
@@ -38543,7 +38543,7 @@
       <c r="A175" s="38" t="s">
         <v>834</v>
       </c>
-      <c r="B175" s="47">
+      <c r="B175" s="42">
         <v>2014</v>
       </c>
       <c r="C175" s="39">
@@ -38566,7 +38566,7 @@
       <c r="A176" s="38" t="s">
         <v>1021</v>
       </c>
-      <c r="B176" s="47">
+      <c r="B176" s="42">
         <v>2018</v>
       </c>
       <c r="C176" s="39">
@@ -38589,7 +38589,7 @@
       <c r="A177" s="38" t="s">
         <v>850</v>
       </c>
-      <c r="B177" s="47">
+      <c r="B177" s="42">
         <v>2014</v>
       </c>
       <c r="C177" s="39">
@@ -38612,7 +38612,7 @@
       <c r="A178" s="38" t="s">
         <v>1027</v>
       </c>
-      <c r="B178" s="47">
+      <c r="B178" s="42">
         <v>2020</v>
       </c>
       <c r="C178" s="39">
@@ -38635,7 +38635,7 @@
       <c r="A179" s="38" t="s">
         <v>351</v>
       </c>
-      <c r="B179" s="47">
+      <c r="B179" s="42">
         <v>2008</v>
       </c>
       <c r="C179" s="39">
@@ -38658,7 +38658,7 @@
       <c r="A180" s="38" t="s">
         <v>485</v>
       </c>
-      <c r="B180" s="47">
+      <c r="B180" s="42">
         <v>2010</v>
       </c>
       <c r="C180" s="39">
@@ -38681,7 +38681,7 @@
       <c r="A181" s="38" t="s">
         <v>627</v>
       </c>
-      <c r="B181" s="47">
+      <c r="B181" s="42">
         <v>2013</v>
       </c>
       <c r="C181" s="39">
@@ -38704,7 +38704,7 @@
       <c r="A182" s="38" t="s">
         <v>937</v>
       </c>
-      <c r="B182" s="47">
+      <c r="B182" s="42">
         <v>2016</v>
       </c>
       <c r="C182" s="39">
@@ -38727,7 +38727,7 @@
       <c r="A183" s="38" t="s">
         <v>440</v>
       </c>
-      <c r="B183" s="47">
+      <c r="B183" s="42">
         <v>2009</v>
       </c>
       <c r="C183" s="39">
@@ -38750,7 +38750,7 @@
       <c r="A184" s="38" t="s">
         <v>1171</v>
       </c>
-      <c r="B184" s="47">
+      <c r="B184" s="42">
         <v>2019</v>
       </c>
       <c r="C184" s="39">
@@ -38773,7 +38773,7 @@
       <c r="A185" s="38" t="s">
         <v>1268</v>
       </c>
-      <c r="B185" s="47">
+      <c r="B185" s="42">
         <v>2022</v>
       </c>
       <c r="C185" s="39">
@@ -38796,7 +38796,7 @@
       <c r="A186" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="B186" s="47">
+      <c r="B186" s="42">
         <v>2008</v>
       </c>
       <c r="C186" s="39">
@@ -38819,7 +38819,7 @@
       <c r="A187" s="38" t="s">
         <v>1198</v>
       </c>
-      <c r="B187" s="47">
+      <c r="B187" s="42">
         <v>2022</v>
       </c>
       <c r="C187" s="39">
@@ -38842,7 +38842,7 @@
       <c r="A188" s="38" t="s">
         <v>1034</v>
       </c>
-      <c r="B188" s="47">
+      <c r="B188" s="42">
         <v>2018</v>
       </c>
       <c r="C188" s="39">
@@ -38865,7 +38865,7 @@
       <c r="A189" s="38" t="s">
         <v>1005</v>
       </c>
-      <c r="B189" s="47">
+      <c r="B189" s="42">
         <v>2018</v>
       </c>
       <c r="C189" s="39">
@@ -38888,7 +38888,7 @@
       <c r="A190" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="B190" s="47">
+      <c r="B190" s="42">
         <v>2007</v>
       </c>
       <c r="C190" s="39">
@@ -38911,7 +38911,7 @@
       <c r="A191" s="38" t="s">
         <v>1106</v>
       </c>
-      <c r="B191" s="47">
+      <c r="B191" s="42">
         <v>2019</v>
       </c>
       <c r="C191" s="39">
@@ -38934,7 +38934,7 @@
       <c r="A192" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B192" s="47">
+      <c r="B192" s="42">
         <v>2005</v>
       </c>
       <c r="C192" s="39">
@@ -38957,7 +38957,7 @@
       <c r="A193" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B193" s="47">
+      <c r="B193" s="42">
         <v>2005</v>
       </c>
       <c r="C193" s="39">
@@ -38980,7 +38980,7 @@
       <c r="A194" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B194" s="47">
+      <c r="B194" s="42">
         <v>2005</v>
       </c>
       <c r="C194" s="39">
@@ -39003,7 +39003,7 @@
       <c r="A195" s="38" t="s">
         <v>1003</v>
       </c>
-      <c r="B195" s="47">
+      <c r="B195" s="42">
         <v>2017</v>
       </c>
       <c r="C195" s="39">
@@ -39026,7 +39026,7 @@
       <c r="A196" s="38" t="s">
         <v>772</v>
       </c>
-      <c r="B196" s="47">
+      <c r="B196" s="42">
         <v>2015</v>
       </c>
       <c r="C196" s="39">
@@ -39049,7 +39049,7 @@
       <c r="A197" s="38" t="s">
         <v>644</v>
       </c>
-      <c r="B197" s="47">
+      <c r="B197" s="42">
         <v>2014</v>
       </c>
       <c r="C197" s="39">
@@ -39072,7 +39072,7 @@
       <c r="A198" s="38" t="s">
         <v>353</v>
       </c>
-      <c r="B198" s="47">
+      <c r="B198" s="42">
         <v>2008</v>
       </c>
       <c r="C198" s="39">
@@ -39095,7 +39095,7 @@
       <c r="A199" s="38" t="s">
         <v>561</v>
       </c>
-      <c r="B199" s="47">
+      <c r="B199" s="42">
         <v>2011</v>
       </c>
       <c r="C199" s="39">
@@ -39118,7 +39118,7 @@
       <c r="A200" s="38" t="s">
         <v>886</v>
       </c>
-      <c r="B200" s="47">
+      <c r="B200" s="42">
         <v>2016</v>
       </c>
       <c r="C200" s="39">
@@ -39141,7 +39141,7 @@
       <c r="A201" s="38" t="s">
         <v>978</v>
       </c>
-      <c r="B201" s="47">
+      <c r="B201" s="42">
         <v>2016</v>
       </c>
       <c r="C201" s="39">
@@ -39164,7 +39164,7 @@
       <c r="A202" s="38" t="s">
         <v>615</v>
       </c>
-      <c r="B202" s="47">
+      <c r="B202" s="42">
         <v>2011</v>
       </c>
       <c r="C202" s="39">
@@ -39187,7 +39187,7 @@
       <c r="A203" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B203" s="47">
+      <c r="B203" s="42">
         <v>2007</v>
       </c>
       <c r="C203" s="39">
@@ -39210,7 +39210,7 @@
       <c r="A204" s="38" t="s">
         <v>552</v>
       </c>
-      <c r="B204" s="47">
+      <c r="B204" s="42">
         <v>2011</v>
       </c>
       <c r="C204" s="39">
@@ -39233,7 +39233,7 @@
       <c r="A205" s="38" t="s">
         <v>703</v>
       </c>
-      <c r="B205" s="47">
+      <c r="B205" s="42">
         <v>2012</v>
       </c>
       <c r="C205" s="39">
@@ -39256,7 +39256,7 @@
       <c r="A206" s="38" t="s">
         <v>547</v>
       </c>
-      <c r="B206" s="47">
+      <c r="B206" s="42">
         <v>2020</v>
       </c>
       <c r="C206" s="39">
@@ -39279,7 +39279,7 @@
       <c r="A207" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="B207" s="47">
+      <c r="B207" s="42">
         <v>2007</v>
       </c>
       <c r="C207" s="39">
@@ -39302,7 +39302,7 @@
       <c r="A208" s="38" t="s">
         <v>1182</v>
       </c>
-      <c r="B208" s="47">
+      <c r="B208" s="42">
         <v>2016</v>
       </c>
       <c r="C208" s="39">
@@ -39325,7 +39325,7 @@
       <c r="A209" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="B209" s="47">
+      <c r="B209" s="42">
         <v>2007</v>
       </c>
       <c r="C209" s="39">
@@ -39348,7 +39348,7 @@
       <c r="A210" s="38" t="s">
         <v>795</v>
       </c>
-      <c r="B210" s="47">
+      <c r="B210" s="42">
         <v>2015</v>
       </c>
       <c r="C210" s="39">
@@ -39371,7 +39371,7 @@
       <c r="A211" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B211" s="47">
+      <c r="B211" s="42">
         <v>2005</v>
       </c>
       <c r="C211" s="39">
@@ -39394,7 +39394,7 @@
       <c r="A212" s="38" t="s">
         <v>1074</v>
       </c>
-      <c r="B212" s="47">
+      <c r="B212" s="42">
         <v>2019</v>
       </c>
       <c r="C212" s="39">
@@ -39417,7 +39417,7 @@
       <c r="A213" s="38" t="s">
         <v>389</v>
       </c>
-      <c r="B213" s="47">
+      <c r="B213" s="42">
         <v>2008</v>
       </c>
       <c r="C213" s="39">
@@ -39440,7 +39440,7 @@
       <c r="A214" s="38" t="s">
         <v>754</v>
       </c>
-      <c r="B214" s="47">
+      <c r="B214" s="42">
         <v>2014</v>
       </c>
       <c r="C214" s="39">
@@ -39463,7 +39463,7 @@
       <c r="A215" s="38" t="s">
         <v>758</v>
       </c>
-      <c r="B215" s="47">
+      <c r="B215" s="42">
         <v>2013</v>
       </c>
       <c r="C215" s="39">
@@ -39486,7 +39486,7 @@
       <c r="A216" s="38" t="s">
         <v>674</v>
       </c>
-      <c r="B216" s="47">
+      <c r="B216" s="42">
         <v>2013</v>
       </c>
       <c r="C216" s="39">
@@ -39509,7 +39509,7 @@
       <c r="A217" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="B217" s="47">
+      <c r="B217" s="42">
         <v>2007</v>
       </c>
       <c r="C217" s="39">
@@ -39532,7 +39532,7 @@
       <c r="A218" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B218" s="47">
+      <c r="B218" s="42">
         <v>2005</v>
       </c>
       <c r="C218" s="39">
@@ -39555,7 +39555,7 @@
       <c r="A219" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B219" s="47">
+      <c r="B219" s="42">
         <v>2005</v>
       </c>
       <c r="C219" s="39">
@@ -39578,7 +39578,7 @@
       <c r="A220" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="B220" s="47">
+      <c r="B220" s="42">
         <v>2005</v>
       </c>
       <c r="C220" s="39">
@@ -39601,7 +39601,7 @@
       <c r="A221" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="B221" s="47">
+      <c r="B221" s="42">
         <v>2006</v>
       </c>
       <c r="C221" s="39">
@@ -39624,7 +39624,7 @@
       <c r="A222" s="38" t="s">
         <v>666</v>
       </c>
-      <c r="B222" s="47">
+      <c r="B222" s="42">
         <v>2012</v>
       </c>
       <c r="C222" s="39">
@@ -39647,7 +39647,7 @@
       <c r="A223" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="B223" s="47">
+      <c r="B223" s="42">
         <v>2006</v>
       </c>
       <c r="C223" s="39">
@@ -39670,7 +39670,7 @@
       <c r="A224" s="38" t="s">
         <v>863</v>
       </c>
-      <c r="B224" s="47">
+      <c r="B224" s="42">
         <v>2015</v>
       </c>
       <c r="C224" s="39">
@@ -39693,7 +39693,7 @@
       <c r="A225" s="38" t="s">
         <v>625</v>
       </c>
-      <c r="B225" s="47">
+      <c r="B225" s="42">
         <v>2011</v>
       </c>
       <c r="C225" s="39">
@@ -39716,7 +39716,7 @@
       <c r="A226" s="38" t="s">
         <v>898</v>
       </c>
-      <c r="B226" s="47">
+      <c r="B226" s="42">
         <v>2017</v>
       </c>
       <c r="C226" s="39">
@@ -39739,7 +39739,7 @@
       <c r="A227" s="38" t="s">
         <v>612</v>
       </c>
-      <c r="B227" s="47">
+      <c r="B227" s="42">
         <v>2012</v>
       </c>
       <c r="C227" s="39">
@@ -39762,7 +39762,7 @@
       <c r="A228" s="38" t="s">
         <v>942</v>
       </c>
-      <c r="B228" s="47">
+      <c r="B228" s="42">
         <v>2017</v>
       </c>
       <c r="C228" s="39">
@@ -39785,7 +39785,7 @@
       <c r="A229" s="38" t="s">
         <v>1192</v>
       </c>
-      <c r="B229" s="47">
+      <c r="B229" s="42">
         <v>2021</v>
       </c>
       <c r="C229" s="39">
@@ -39808,7 +39808,7 @@
       <c r="A230" s="38" t="s">
         <v>799</v>
       </c>
-      <c r="B230" s="47">
+      <c r="B230" s="42">
         <v>2015</v>
       </c>
       <c r="C230" s="39">
@@ -39831,7 +39831,7 @@
       <c r="A231" s="38" t="s">
         <v>1194</v>
       </c>
-      <c r="B231" s="47">
+      <c r="B231" s="42">
         <v>2022</v>
       </c>
       <c r="C231" s="39">
@@ -39854,7 +39854,7 @@
       <c r="A232" s="38" t="s">
         <v>701</v>
       </c>
-      <c r="B232" s="47">
+      <c r="B232" s="42">
         <v>2013</v>
       </c>
       <c r="C232" s="39">
@@ -39877,7 +39877,7 @@
       <c r="A233" s="38" t="s">
         <v>285</v>
       </c>
-      <c r="B233" s="47">
+      <c r="B233" s="42">
         <v>2007</v>
       </c>
       <c r="C233" s="39">
@@ -39900,7 +39900,7 @@
       <c r="A234" s="38" t="s">
         <v>710</v>
       </c>
-      <c r="B234" s="47">
+      <c r="B234" s="42">
         <v>2014</v>
       </c>
       <c r="C234" s="39">
@@ -39923,7 +39923,7 @@
       <c r="A235" s="38" t="s">
         <v>956</v>
       </c>
-      <c r="B235" s="47">
+      <c r="B235" s="42">
         <v>2016</v>
       </c>
       <c r="C235" s="39">
@@ -39946,7 +39946,7 @@
       <c r="A236" s="38" t="s">
         <v>916</v>
       </c>
-      <c r="B236" s="47">
+      <c r="B236" s="42">
         <v>2015</v>
       </c>
       <c r="C236" s="39">
@@ -39969,7 +39969,7 @@
       <c r="A237" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="B237" s="47">
+      <c r="B237" s="42">
         <v>2006</v>
       </c>
       <c r="C237" s="39">
@@ -39992,7 +39992,7 @@
       <c r="A238" s="38" t="s">
         <v>581</v>
       </c>
-      <c r="B238" s="47">
+      <c r="B238" s="42">
         <v>2011</v>
       </c>
       <c r="C238" s="39">
@@ -40015,7 +40015,7 @@
       <c r="A239" s="38" t="s">
         <v>1162</v>
       </c>
-      <c r="B239" s="47">
+      <c r="B239" s="42">
         <v>2021</v>
       </c>
       <c r="C239" s="39">
@@ -40038,7 +40038,7 @@
       <c r="A240" s="38" t="s">
         <v>1056</v>
       </c>
-      <c r="B240" s="47">
+      <c r="B240" s="42">
         <v>2018</v>
       </c>
       <c r="C240" s="39">
@@ -40061,7 +40061,7 @@
       <c r="A241" s="38" t="s">
         <v>498</v>
       </c>
-      <c r="B241" s="47">
+      <c r="B241" s="42">
         <v>2010</v>
       </c>
       <c r="C241" s="39">
@@ -40084,7 +40084,7 @@
       <c r="A242" s="38" t="s">
         <v>1098</v>
       </c>
-      <c r="B242" s="47">
+      <c r="B242" s="42">
         <v>2020</v>
       </c>
       <c r="C242" s="39">
@@ -40107,7 +40107,7 @@
       <c r="A243" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="B243" s="47">
+      <c r="B243" s="42">
         <v>2005</v>
       </c>
       <c r="C243" s="39">
@@ -40130,7 +40130,7 @@
       <c r="A244" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="B244" s="47">
+      <c r="B244" s="42">
         <v>2006</v>
       </c>
       <c r="C244" s="39">
@@ -40153,7 +40153,7 @@
       <c r="A245" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B245" s="48">
+      <c r="B245" s="43">
         <v>2004</v>
       </c>
       <c r="C245" s="37">
@@ -40176,7 +40176,7 @@
       <c r="A246" s="38" t="s">
         <v>413</v>
       </c>
-      <c r="B246" s="47">
+      <c r="B246" s="42">
         <v>2009</v>
       </c>
       <c r="C246" s="39">
@@ -40199,7 +40199,7 @@
       <c r="A247" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B247" s="48">
+      <c r="B247" s="43">
         <v>2004</v>
       </c>
       <c r="C247" s="37">
@@ -40222,7 +40222,7 @@
       <c r="A248" s="38" t="s">
         <v>782</v>
       </c>
-      <c r="B248" s="47">
+      <c r="B248" s="42">
         <v>2014</v>
       </c>
       <c r="C248" s="39">
@@ -40245,7 +40245,7 @@
       <c r="A249" s="38" t="s">
         <v>816</v>
       </c>
-      <c r="B249" s="47">
+      <c r="B249" s="42">
         <v>2014</v>
       </c>
       <c r="C249" s="39">
@@ -40268,7 +40268,7 @@
       <c r="A250" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="B250" s="47">
+      <c r="B250" s="42">
         <v>2006</v>
       </c>
       <c r="C250" s="39">
@@ -40291,7 +40291,7 @@
       <c r="A251" s="38" t="s">
         <v>398</v>
       </c>
-      <c r="B251" s="47">
+      <c r="B251" s="42">
         <v>2008</v>
       </c>
       <c r="C251" s="39">
@@ -40314,7 +40314,7 @@
       <c r="A252" s="38" t="s">
         <v>605</v>
       </c>
-      <c r="B252" s="47">
+      <c r="B252" s="42">
         <v>2012</v>
       </c>
       <c r="C252" s="39">
@@ -40337,7 +40337,7 @@
       <c r="A253" s="38" t="s">
         <v>966</v>
       </c>
-      <c r="B253" s="47">
+      <c r="B253" s="42">
         <v>2017</v>
       </c>
       <c r="C253" s="39">
@@ -40360,7 +40360,7 @@
       <c r="A254" s="38" t="s">
         <v>669</v>
       </c>
-      <c r="B254" s="47">
+      <c r="B254" s="42">
         <v>2013</v>
       </c>
       <c r="C254" s="39">
@@ -40383,7 +40383,7 @@
       <c r="A255" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="B255" s="47">
+      <c r="B255" s="42">
         <v>2006</v>
       </c>
       <c r="C255" s="39">
@@ -40406,7 +40406,7 @@
       <c r="A256" s="38" t="s">
         <v>448</v>
       </c>
-      <c r="B256" s="47">
+      <c r="B256" s="42">
         <v>2009</v>
       </c>
       <c r="C256" s="39">
@@ -40429,7 +40429,7 @@
       <c r="A257" s="38" t="s">
         <v>807</v>
       </c>
-      <c r="B257" s="47">
+      <c r="B257" s="42">
         <v>2014</v>
       </c>
       <c r="C257" s="39">
@@ -40452,7 +40452,7 @@
       <c r="A258" s="38" t="s">
         <v>722</v>
       </c>
-      <c r="B258" s="47">
+      <c r="B258" s="42">
         <v>2015</v>
       </c>
       <c r="C258" s="39">
@@ -40475,7 +40475,7 @@
       <c r="A259" s="38" t="s">
         <v>1196</v>
       </c>
-      <c r="B259" s="47">
+      <c r="B259" s="42">
         <v>2021</v>
       </c>
       <c r="C259" s="39">
@@ -40498,7 +40498,7 @@
       <c r="A260" s="38" t="s">
         <v>765</v>
       </c>
-      <c r="B260" s="47">
+      <c r="B260" s="42">
         <v>2013</v>
       </c>
       <c r="C260" s="39">
@@ -40521,7 +40521,7 @@
       <c r="A261" s="38" t="s">
         <v>855</v>
       </c>
-      <c r="B261" s="47">
+      <c r="B261" s="42">
         <v>2016</v>
       </c>
       <c r="C261" s="39">
@@ -40544,7 +40544,7 @@
       <c r="A262" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="B262" s="47">
+      <c r="B262" s="42">
         <v>2007</v>
       </c>
       <c r="C262" s="39">
@@ -40567,7 +40567,7 @@
       <c r="A263" s="38" t="s">
         <v>756</v>
       </c>
-      <c r="B263" s="47">
+      <c r="B263" s="42">
         <v>2014</v>
       </c>
       <c r="C263" s="39">
@@ -40590,7 +40590,7 @@
       <c r="A264" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="B264" s="47">
+      <c r="B264" s="42">
         <v>2006</v>
       </c>
       <c r="C264" s="39">
@@ -40613,7 +40613,7 @@
       <c r="A265" s="38" t="s">
         <v>1169</v>
       </c>
-      <c r="B265" s="47">
+      <c r="B265" s="42">
         <v>2020</v>
       </c>
       <c r="C265" s="39">
@@ -40636,7 +40636,7 @@
       <c r="A266" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="B266" s="47">
+      <c r="B266" s="42">
         <v>2009</v>
       </c>
       <c r="C266" s="39">
@@ -40659,7 +40659,7 @@
       <c r="A267" s="38" t="s">
         <v>890</v>
       </c>
-      <c r="B267" s="47">
+      <c r="B267" s="42">
         <v>2018</v>
       </c>
       <c r="C267" s="39">
@@ -40682,7 +40682,7 @@
       <c r="A268" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="B268" s="47">
+      <c r="B268" s="42">
         <v>2008</v>
       </c>
       <c r="C268" s="39">
@@ -40705,7 +40705,7 @@
       <c r="A269" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="B269" s="47">
+      <c r="B269" s="42">
         <v>2008</v>
       </c>
       <c r="C269" s="39">
@@ -40728,7 +40728,7 @@
       <c r="A270" s="38" t="s">
         <v>904</v>
       </c>
-      <c r="B270" s="47">
+      <c r="B270" s="42">
         <v>2016</v>
       </c>
       <c r="C270" s="39">
@@ -40751,7 +40751,7 @@
       <c r="A271" s="38" t="s">
         <v>749</v>
       </c>
-      <c r="B271" s="47">
+      <c r="B271" s="42">
         <v>2013</v>
       </c>
       <c r="C271" s="39">
@@ -40774,7 +40774,7 @@
       <c r="A272" s="38" t="s">
         <v>896</v>
       </c>
-      <c r="B272" s="47">
+      <c r="B272" s="42">
         <v>2016</v>
       </c>
       <c r="C272" s="39">
@@ -40797,7 +40797,7 @@
       <c r="A273" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="B273" s="47">
+      <c r="B273" s="42">
         <v>2007</v>
       </c>
       <c r="C273" s="39">
@@ -40820,7 +40820,7 @@
       <c r="A274" s="38" t="s">
         <v>1070</v>
       </c>
-      <c r="B274" s="47">
+      <c r="B274" s="42">
         <v>2019</v>
       </c>
       <c r="C274" s="39">
@@ -40843,7 +40843,7 @@
       <c r="A275" s="38" t="s">
         <v>1165</v>
       </c>
-      <c r="B275" s="47">
+      <c r="B275" s="42">
         <v>2020</v>
       </c>
       <c r="C275" s="39">
@@ -40866,7 +40866,7 @@
       <c r="A276" s="38" t="s">
         <v>1235</v>
       </c>
-      <c r="B276" s="47">
+      <c r="B276" s="42">
         <v>2019</v>
       </c>
       <c r="C276" s="39">
@@ -40889,7 +40889,7 @@
       <c r="A277" s="38" t="s">
         <v>1130</v>
       </c>
-      <c r="B277" s="47">
+      <c r="B277" s="42">
         <v>2020</v>
       </c>
       <c r="C277" s="39">
@@ -40912,7 +40912,7 @@
       <c r="A278" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="B278" s="47">
+      <c r="B278" s="42">
         <v>2010</v>
       </c>
       <c r="C278" s="39">
@@ -40935,7 +40935,7 @@
       <c r="A279" s="38" t="s">
         <v>1110</v>
       </c>
-      <c r="B279" s="47">
+      <c r="B279" s="42">
         <v>2021</v>
       </c>
       <c r="C279" s="39">
@@ -40958,7 +40958,7 @@
       <c r="A280" s="38" t="s">
         <v>526</v>
       </c>
-      <c r="B280" s="47">
+      <c r="B280" s="42">
         <v>2010</v>
       </c>
       <c r="C280" s="39">
@@ -40981,7 +40981,7 @@
       <c r="A281" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="B281" s="47">
+      <c r="B281" s="42">
         <v>2007</v>
       </c>
       <c r="C281" s="39">
@@ -41004,7 +41004,7 @@
       <c r="A282" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="B282" s="47">
+      <c r="B282" s="42">
         <v>2006</v>
       </c>
       <c r="C282" s="39">
@@ -41027,7 +41027,7 @@
       <c r="A283" s="38" t="s">
         <v>991</v>
       </c>
-      <c r="B283" s="47">
+      <c r="B283" s="42">
         <v>2017</v>
       </c>
       <c r="C283" s="39">
@@ -41050,7 +41050,7 @@
       <c r="A284" s="38" t="s">
         <v>556</v>
       </c>
-      <c r="B284" s="47">
+      <c r="B284" s="42">
         <v>2011</v>
       </c>
       <c r="C284" s="39">
@@ -41073,7 +41073,7 @@
       <c r="A285" s="38" t="s">
         <v>402</v>
       </c>
-      <c r="B285" s="47">
+      <c r="B285" s="42">
         <v>2008</v>
       </c>
       <c r="C285" s="39">
@@ -41096,7 +41096,7 @@
       <c r="A286" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="B286" s="47">
+      <c r="B286" s="42">
         <v>2006</v>
       </c>
       <c r="C286" s="39">
@@ -41119,7 +41119,7 @@
       <c r="A287" s="38" t="s">
         <v>496</v>
       </c>
-      <c r="B287" s="47">
+      <c r="B287" s="42">
         <v>2010</v>
       </c>
       <c r="C287" s="39">
@@ -41142,7 +41142,7 @@
       <c r="A288" s="38" t="s">
         <v>356</v>
       </c>
-      <c r="B288" s="47">
+      <c r="B288" s="42">
         <v>2008</v>
       </c>
       <c r="C288" s="39">
@@ -41165,7 +41165,7 @@
       <c r="A289" s="38" t="s">
         <v>587</v>
       </c>
-      <c r="B289" s="47">
+      <c r="B289" s="42">
         <v>2011</v>
       </c>
       <c r="C289" s="39">
@@ -41188,7 +41188,7 @@
       <c r="A290" s="38" t="s">
         <v>609</v>
       </c>
-      <c r="B290" s="47">
+      <c r="B290" s="42">
         <v>2012</v>
       </c>
       <c r="C290" s="39">
@@ -41211,7 +41211,7 @@
       <c r="A291" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="B291" s="47">
+      <c r="B291" s="42">
         <v>2008</v>
       </c>
       <c r="C291" s="39">
@@ -41234,7 +41234,7 @@
       <c r="A292" s="38" t="s">
         <v>554</v>
       </c>
-      <c r="B292" s="47">
+      <c r="B292" s="42">
         <v>2011</v>
       </c>
       <c r="C292" s="39">
@@ -41257,7 +41257,7 @@
       <c r="A293" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B293" s="48">
+      <c r="B293" s="43">
         <v>2004</v>
       </c>
       <c r="C293" s="37">
@@ -41280,7 +41280,7 @@
       <c r="A294" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="B294" s="47">
+      <c r="B294" s="42">
         <v>2006</v>
       </c>
       <c r="C294" s="39">
@@ -41303,7 +41303,7 @@
       <c r="A295" s="38" t="s">
         <v>578</v>
       </c>
-      <c r="B295" s="47">
+      <c r="B295" s="42">
         <v>2011</v>
       </c>
       <c r="C295" s="39">
@@ -41326,7 +41326,7 @@
       <c r="A296" s="38" t="s">
         <v>366</v>
       </c>
-      <c r="B296" s="47">
+      <c r="B296" s="42">
         <v>2008</v>
       </c>
       <c r="C296" s="39">
@@ -41349,7 +41349,7 @@
       <c r="A297" s="38" t="s">
         <v>427</v>
       </c>
-      <c r="B297" s="47">
+      <c r="B297" s="42">
         <v>2009</v>
       </c>
       <c r="C297" s="39">
@@ -41372,7 +41372,7 @@
       <c r="A298" s="38" t="s">
         <v>751</v>
       </c>
-      <c r="B298" s="47">
+      <c r="B298" s="42">
         <v>2013</v>
       </c>
       <c r="C298" s="39">
@@ -41395,7 +41395,7 @@
       <c r="A299" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="B299" s="47">
+      <c r="B299" s="42">
         <v>2006</v>
       </c>
       <c r="C299" s="39">
@@ -41418,7 +41418,7 @@
       <c r="A300" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B300" s="48">
+      <c r="B300" s="43">
         <v>2004</v>
       </c>
       <c r="C300" s="37">
@@ -41441,7 +41441,7 @@
       <c r="A301" s="38" t="s">
         <v>570</v>
       </c>
-      <c r="B301" s="47">
+      <c r="B301" s="42">
         <v>2011</v>
       </c>
       <c r="C301" s="39">
@@ -41464,7 +41464,7 @@
       <c r="A302" s="38" t="s">
         <v>487</v>
       </c>
-      <c r="B302" s="47">
+      <c r="B302" s="42">
         <v>2010</v>
       </c>
       <c r="C302" s="39">
@@ -41487,7 +41487,7 @@
       <c r="A303" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="B303" s="48">
+      <c r="B303" s="43">
         <v>2004</v>
       </c>
       <c r="C303" s="37">
@@ -41510,7 +41510,7 @@
       <c r="A304" s="38" t="s">
         <v>392</v>
       </c>
-      <c r="B304" s="47">
+      <c r="B304" s="42">
         <v>2008</v>
       </c>
       <c r="C304" s="39">
@@ -41533,7 +41533,7 @@
       <c r="A305" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="B305" s="47">
+      <c r="B305" s="42">
         <v>2005</v>
       </c>
       <c r="C305" s="39">
@@ -41556,7 +41556,7 @@
       <c r="A306" s="38" t="s">
         <v>451</v>
       </c>
-      <c r="B306" s="47">
+      <c r="B306" s="42">
         <v>2009</v>
       </c>
       <c r="C306" s="39">
@@ -41579,7 +41579,7 @@
       <c r="A307" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B307" s="48">
+      <c r="B307" s="43">
         <v>2004</v>
       </c>
       <c r="C307" s="37">
@@ -41602,7 +41602,7 @@
       <c r="A308" s="38" t="s">
         <v>515</v>
       </c>
-      <c r="B308" s="47">
+      <c r="B308" s="42">
         <v>2010</v>
       </c>
       <c r="C308" s="39">
@@ -41625,7 +41625,7 @@
       <c r="A309" s="38" t="s">
         <v>1154</v>
       </c>
-      <c r="B309" s="47">
+      <c r="B309" s="42">
         <v>2020</v>
       </c>
       <c r="C309" s="39">
@@ -41648,7 +41648,7 @@
       <c r="A310" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="B310" s="47">
+      <c r="B310" s="42">
         <v>2008</v>
       </c>
       <c r="C310" s="39">
@@ -41671,7 +41671,7 @@
       <c r="A311" s="38" t="s">
         <v>1087</v>
       </c>
-      <c r="B311" s="47">
+      <c r="B311" s="42">
         <v>2018</v>
       </c>
       <c r="C311" s="39">
@@ -41694,7 +41694,7 @@
       <c r="A312" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="B312" s="47">
+      <c r="B312" s="42">
         <v>2010</v>
       </c>
       <c r="C312" s="39">
@@ -41717,7 +41717,7 @@
       <c r="A313" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="B313" s="47">
+      <c r="B313" s="42">
         <v>2007</v>
       </c>
       <c r="C313" s="39">
@@ -41740,7 +41740,7 @@
       <c r="A314" s="38" t="s">
         <v>1066</v>
       </c>
-      <c r="B314" s="47">
+      <c r="B314" s="42">
         <v>2020</v>
       </c>
       <c r="C314" s="39">
@@ -41763,7 +41763,7 @@
       <c r="A315" s="38" t="s">
         <v>695</v>
       </c>
-      <c r="B315" s="47">
+      <c r="B315" s="42">
         <v>2013</v>
       </c>
       <c r="C315" s="39">
@@ -41786,7 +41786,7 @@
       <c r="A316" s="38" t="s">
         <v>620</v>
       </c>
-      <c r="B316" s="47">
+      <c r="B316" s="42">
         <v>2011</v>
       </c>
       <c r="C316" s="39">
@@ -41809,7 +41809,7 @@
       <c r="A317" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="B317" s="47">
+      <c r="B317" s="42">
         <v>2007</v>
       </c>
       <c r="C317" s="39">
@@ -41832,7 +41832,7 @@
       <c r="A318" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="B318" s="47">
+      <c r="B318" s="42">
         <v>2007</v>
       </c>
       <c r="C318" s="39">
@@ -41855,7 +41855,7 @@
       <c r="A319" s="38" t="s">
         <v>1246</v>
       </c>
-      <c r="B319" s="47">
+      <c r="B319" s="42">
         <v>2021</v>
       </c>
       <c r="C319" s="39">
@@ -41878,7 +41878,7 @@
       <c r="A320" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B320" s="47">
+      <c r="B320" s="42">
         <v>2005</v>
       </c>
       <c r="C320" s="39">
@@ -41901,7 +41901,7 @@
       <c r="A321" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="B321" s="47">
+      <c r="B321" s="42">
         <v>2007</v>
       </c>
       <c r="C321" s="39">
@@ -41924,7 +41924,7 @@
       <c r="A322" s="38" t="s">
         <v>509</v>
       </c>
-      <c r="B322" s="47">
+      <c r="B322" s="42">
         <v>2010</v>
       </c>
       <c r="C322" s="39">
@@ -41947,7 +41947,7 @@
       <c r="A323" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="B323" s="48">
+      <c r="B323" s="43">
         <v>2004</v>
       </c>
       <c r="C323" s="37">
@@ -41970,7 +41970,7 @@
       <c r="A324" s="38" t="s">
         <v>585</v>
       </c>
-      <c r="B324" s="47">
+      <c r="B324" s="42">
         <v>2011</v>
       </c>
       <c r="C324" s="39">
@@ -41993,7 +41993,7 @@
       <c r="A325" s="38" t="s">
         <v>1264</v>
       </c>
-      <c r="B325" s="47">
+      <c r="B325" s="42">
         <v>2022</v>
       </c>
       <c r="C325" s="39">
@@ -42016,7 +42016,7 @@
       <c r="A326" s="38" t="s">
         <v>595</v>
       </c>
-      <c r="B326" s="47">
+      <c r="B326" s="42">
         <v>2012</v>
       </c>
       <c r="C326" s="39">
@@ -42039,7 +42039,7 @@
       <c r="A327" s="38" t="s">
         <v>698</v>
       </c>
-      <c r="B327" s="47">
+      <c r="B327" s="42">
         <v>2013</v>
       </c>
       <c r="C327" s="39">
@@ -42062,7 +42062,7 @@
       <c r="A328" s="38" t="s">
         <v>1202</v>
       </c>
-      <c r="B328" s="47">
+      <c r="B328" s="42">
         <v>2021</v>
       </c>
       <c r="C328" s="39">
@@ -42085,7 +42085,7 @@
       <c r="A329" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="B329" s="47">
+      <c r="B329" s="42">
         <v>2011</v>
       </c>
       <c r="C329" s="39">
@@ -42108,7 +42108,7 @@
       <c r="A330" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B330" s="48">
+      <c r="B330" s="43">
         <v>2004</v>
       </c>
       <c r="C330" s="37">
@@ -42131,7 +42131,7 @@
       <c r="A331" s="38" t="s">
         <v>1146</v>
       </c>
-      <c r="B331" s="47">
+      <c r="B331" s="42">
         <v>2019</v>
       </c>
       <c r="C331" s="39">
@@ -42154,7 +42154,7 @@
       <c r="A332" s="38" t="s">
         <v>973</v>
       </c>
-      <c r="B332" s="47">
+      <c r="B332" s="42">
         <v>2017</v>
       </c>
       <c r="C332" s="39">
@@ -42177,7 +42177,7 @@
       <c r="A333" s="38" t="s">
         <v>1217</v>
       </c>
-      <c r="B333" s="47">
+      <c r="B333" s="42">
         <v>2021</v>
       </c>
       <c r="C333" s="39">
@@ -42200,7 +42200,7 @@
       <c r="A334" s="38" t="s">
         <v>1123</v>
       </c>
-      <c r="B334" s="47">
+      <c r="B334" s="42">
         <v>2020</v>
       </c>
       <c r="C334" s="39">
@@ -42223,7 +42223,7 @@
       <c r="A335" s="38" t="s">
         <v>1140</v>
       </c>
-      <c r="B335" s="47">
+      <c r="B335" s="42">
         <v>2021</v>
       </c>
       <c r="C335" s="39">
@@ -42246,7 +42246,7 @@
       <c r="A336" s="38" t="s">
         <v>948</v>
       </c>
-      <c r="B336" s="47">
+      <c r="B336" s="42">
         <v>2022</v>
       </c>
       <c r="C336" s="39">
@@ -42269,7 +42269,7 @@
       <c r="A337" s="38" t="s">
         <v>894</v>
       </c>
-      <c r="B337" s="47">
+      <c r="B337" s="42">
         <v>2015</v>
       </c>
       <c r="C337" s="39">
@@ -42292,7 +42292,7 @@
       <c r="A338" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B338" s="47">
+      <c r="B338" s="42">
         <v>2005</v>
       </c>
       <c r="C338" s="39">
@@ -42315,7 +42315,7 @@
       <c r="A339" s="38" t="s">
         <v>1136</v>
       </c>
-      <c r="B339" s="47">
+      <c r="B339" s="42">
         <v>2020</v>
       </c>
       <c r="C339" s="39">
@@ -42338,7 +42338,7 @@
       <c r="A340" s="38" t="s">
         <v>1160</v>
       </c>
-      <c r="B340" s="47">
+      <c r="B340" s="42">
         <v>2019</v>
       </c>
       <c r="C340" s="39">
@@ -42361,7 +42361,7 @@
       <c r="A341" s="38" t="s">
         <v>983</v>
       </c>
-      <c r="B341" s="47">
+      <c r="B341" s="42">
         <v>2017</v>
       </c>
       <c r="C341" s="39">
@@ -42384,7 +42384,7 @@
       <c r="A342" s="38" t="s">
         <v>1144</v>
       </c>
-      <c r="B342" s="47">
+      <c r="B342" s="42">
         <v>2020</v>
       </c>
       <c r="C342" s="39">
@@ -42407,7 +42407,7 @@
       <c r="A343" s="38" t="s">
         <v>919</v>
       </c>
-      <c r="B343" s="47">
+      <c r="B343" s="42">
         <v>2006</v>
       </c>
       <c r="C343" s="39">
@@ -42430,7 +42430,7 @@
       <c r="A344" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="B344" s="47">
+      <c r="B344" s="42">
         <v>2006</v>
       </c>
       <c r="C344" s="39">
@@ -42453,7 +42453,7 @@
       <c r="A345" s="38" t="s">
         <v>359</v>
       </c>
-      <c r="B345" s="47">
+      <c r="B345" s="42">
         <v>2008</v>
       </c>
       <c r="C345" s="39">
@@ -42476,7 +42476,7 @@
       <c r="A346" s="38" t="s">
         <v>549</v>
       </c>
-      <c r="B346" s="47">
+      <c r="B346" s="42">
         <v>2011</v>
       </c>
       <c r="C346" s="39">
@@ -42499,7 +42499,7 @@
       <c r="A347" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="B347" s="47">
+      <c r="B347" s="42">
         <v>2006</v>
       </c>
       <c r="C347" s="39">
@@ -42522,7 +42522,7 @@
       <c r="A348" s="38" t="s">
         <v>1023</v>
       </c>
-      <c r="B348" s="47">
+      <c r="B348" s="42">
         <v>2019</v>
       </c>
       <c r="C348" s="39">
@@ -42545,7 +42545,7 @@
       <c r="A349" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="B349" s="47">
+      <c r="B349" s="42">
         <v>2005</v>
       </c>
       <c r="C349" s="39">
@@ -42568,7 +42568,7 @@
       <c r="A350" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="B350" s="48">
+      <c r="B350" s="43">
         <v>2004</v>
       </c>
       <c r="C350" s="37">
@@ -42591,7 +42591,7 @@
       <c r="A351" s="38" t="s">
         <v>456</v>
       </c>
-      <c r="B351" s="47">
+      <c r="B351" s="42">
         <v>2009</v>
       </c>
       <c r="C351" s="39">
@@ -42614,7 +42614,7 @@
       <c r="A352" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B352" s="47">
+      <c r="B352" s="42">
         <v>2008</v>
       </c>
       <c r="C352" s="39">
@@ -42637,7 +42637,7 @@
       <c r="A353" s="38" t="s">
         <v>705</v>
       </c>
-      <c r="B353" s="47">
+      <c r="B353" s="42">
         <v>2012</v>
       </c>
       <c r="C353" s="39">
@@ -42660,7 +42660,7 @@
       <c r="A354" s="38" t="s">
         <v>1083</v>
       </c>
-      <c r="B354" s="47">
+      <c r="B354" s="42">
         <v>2019</v>
       </c>
       <c r="C354" s="39">
@@ -42683,7 +42683,7 @@
       <c r="A355" s="38" t="s">
         <v>726</v>
       </c>
-      <c r="B355" s="47">
+      <c r="B355" s="42">
         <v>2014</v>
       </c>
       <c r="C355" s="39">
@@ -42706,7 +42706,7 @@
       <c r="A356" s="38" t="s">
         <v>906</v>
       </c>
-      <c r="B356" s="47">
+      <c r="B356" s="42">
         <v>2010</v>
       </c>
       <c r="C356" s="39">
@@ -42729,7 +42729,7 @@
       <c r="A357" s="38" t="s">
         <v>1176</v>
       </c>
-      <c r="B357" s="47">
+      <c r="B357" s="42">
         <v>2020</v>
       </c>
       <c r="C357" s="39">
@@ -42752,7 +42752,7 @@
       <c r="A358" s="36" t="s">
         <v>981</v>
       </c>
-      <c r="B358" s="48">
+      <c r="B358" s="43">
         <v>2004</v>
       </c>
       <c r="C358" s="37">
@@ -42775,7 +42775,7 @@
       <c r="A359" s="38" t="s">
         <v>785</v>
       </c>
-      <c r="B359" s="47">
+      <c r="B359" s="42">
         <v>2015</v>
       </c>
       <c r="C359" s="39">
@@ -42798,7 +42798,7 @@
       <c r="A360" s="38" t="s">
         <v>446</v>
       </c>
-      <c r="B360" s="47">
+      <c r="B360" s="42">
         <v>2009</v>
       </c>
       <c r="C360" s="39">
@@ -42821,7 +42821,7 @@
       <c r="A361" s="38" t="s">
         <v>1112</v>
       </c>
-      <c r="B361" s="47">
+      <c r="B361" s="42">
         <v>2019</v>
       </c>
       <c r="C361" s="39">
@@ -42844,7 +42844,7 @@
       <c r="A362" s="38" t="s">
         <v>909</v>
       </c>
-      <c r="B362" s="47">
+      <c r="B362" s="42">
         <v>2015</v>
       </c>
       <c r="C362" s="39">
@@ -42867,7 +42867,7 @@
       <c r="A363" s="38" t="s">
         <v>1030</v>
       </c>
-      <c r="B363" s="47">
+      <c r="B363" s="42">
         <v>2018</v>
       </c>
       <c r="C363" s="39">
@@ -42890,7 +42890,7 @@
       <c r="A364" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="B364" s="47">
+      <c r="B364" s="42">
         <v>2014</v>
       </c>
       <c r="C364" s="39">
@@ -42913,7 +42913,7 @@
       <c r="A365" s="38" t="s">
         <v>930</v>
       </c>
-      <c r="B365" s="47">
+      <c r="B365" s="42">
         <v>2016</v>
       </c>
       <c r="C365" s="39">
@@ -42936,7 +42936,7 @@
       <c r="A366" s="38" t="s">
         <v>688</v>
       </c>
-      <c r="B366" s="47">
+      <c r="B366" s="42">
         <v>2012</v>
       </c>
       <c r="C366" s="39">
@@ -42959,7 +42959,7 @@
       <c r="A367" s="38" t="s">
         <v>734</v>
       </c>
-      <c r="B367" s="47">
+      <c r="B367" s="42">
         <v>2014</v>
       </c>
       <c r="C367" s="39">
@@ -42982,7 +42982,7 @@
       <c r="A368" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="B368" s="47">
+      <c r="B368" s="42">
         <v>2005</v>
       </c>
       <c r="C368" s="39">
@@ -43005,7 +43005,7 @@
       <c r="A369" s="38" t="s">
         <v>724</v>
       </c>
-      <c r="B369" s="47">
+      <c r="B369" s="42">
         <v>2013</v>
       </c>
       <c r="C369" s="39">
@@ -43028,7 +43028,7 @@
       <c r="A370" s="38" t="s">
         <v>671</v>
       </c>
-      <c r="B370" s="47">
+      <c r="B370" s="42">
         <v>2012</v>
       </c>
       <c r="C370" s="39">
@@ -43051,7 +43051,7 @@
       <c r="A371" s="38" t="s">
         <v>821</v>
       </c>
-      <c r="B371" s="47">
+      <c r="B371" s="42">
         <v>2015</v>
       </c>
       <c r="C371" s="39">
@@ -43074,7 +43074,7 @@
       <c r="A372" s="38" t="s">
         <v>1101</v>
       </c>
-      <c r="B372" s="47">
+      <c r="B372" s="42">
         <v>2019</v>
       </c>
       <c r="C372" s="39">
@@ -43097,7 +43097,7 @@
       <c r="A373" s="38" t="s">
         <v>638</v>
       </c>
-      <c r="B373" s="47">
+      <c r="B373" s="42">
         <v>2009</v>
       </c>
       <c r="C373" s="39">
@@ -43120,7 +43120,7 @@
       <c r="A374" s="38" t="s">
         <v>1233</v>
       </c>
-      <c r="B374" s="47">
+      <c r="B374" s="42">
         <v>2022</v>
       </c>
       <c r="C374" s="39">
@@ -43143,7 +43143,7 @@
       <c r="A375" s="38" t="s">
         <v>1076</v>
       </c>
-      <c r="B375" s="47">
+      <c r="B375" s="42">
         <v>2019</v>
       </c>
       <c r="C375" s="39">
@@ -43166,7 +43166,7 @@
       <c r="A376" s="38" t="s">
         <v>932</v>
       </c>
-      <c r="B376" s="47">
+      <c r="B376" s="42">
         <v>2017</v>
       </c>
       <c r="C376" s="39">
@@ -43189,7 +43189,7 @@
       <c r="A377" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B377" s="47">
+      <c r="B377" s="42">
         <v>2005</v>
       </c>
       <c r="C377" s="39">
@@ -43212,7 +43212,7 @@
       <c r="A378" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B378" s="48">
+      <c r="B378" s="43">
         <v>2004</v>
       </c>
       <c r="C378" s="37">
@@ -43235,7 +43235,7 @@
       <c r="A379" s="38" t="s">
         <v>996</v>
       </c>
-      <c r="B379" s="47">
+      <c r="B379" s="42">
         <v>2017</v>
       </c>
       <c r="C379" s="39">
@@ -43258,7 +43258,7 @@
       <c r="A380" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="B380" s="47">
+      <c r="B380" s="42">
         <v>2007</v>
       </c>
       <c r="C380" s="39">
@@ -43281,7 +43281,7 @@
       <c r="A381" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B381" s="48">
+      <c r="B381" s="43">
         <v>2004</v>
       </c>
       <c r="C381" s="37">
@@ -43304,7 +43304,7 @@
       <c r="A382" s="38" t="s">
         <v>842</v>
       </c>
-      <c r="B382" s="47">
+      <c r="B382" s="42">
         <v>2015</v>
       </c>
       <c r="C382" s="39">
@@ -43327,7 +43327,7 @@
       <c r="A383" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="B383" s="47">
+      <c r="B383" s="42">
         <v>2005</v>
       </c>
       <c r="C383" s="39">
@@ -43350,7 +43350,7 @@
       <c r="A384" s="38" t="s">
         <v>829</v>
       </c>
-      <c r="B384" s="47">
+      <c r="B384" s="42">
         <v>2015</v>
       </c>
       <c r="C384" s="39">
@@ -43373,7 +43373,7 @@
       <c r="A385" s="38" t="s">
         <v>566</v>
       </c>
-      <c r="B385" s="47">
+      <c r="B385" s="42">
         <v>2011</v>
       </c>
       <c r="C385" s="39">
@@ -43396,7 +43396,7 @@
       <c r="A386" s="38" t="s">
         <v>598</v>
       </c>
-      <c r="B386" s="47">
+      <c r="B386" s="42">
         <v>2012</v>
       </c>
       <c r="C386" s="39">
@@ -43419,7 +43419,7 @@
       <c r="A387" s="38" t="s">
         <v>1244</v>
       </c>
-      <c r="B387" s="47">
+      <c r="B387" s="42">
         <v>2021</v>
       </c>
       <c r="C387" s="39">
@@ -43442,7 +43442,7 @@
       <c r="A388" s="38" t="s">
         <v>430</v>
       </c>
-      <c r="B388" s="47">
+      <c r="B388" s="42">
         <v>2009</v>
       </c>
       <c r="C388" s="39">
@@ -43465,7 +43465,7 @@
       <c r="A389" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="B389" s="47">
+      <c r="B389" s="42">
         <v>2006</v>
       </c>
       <c r="C389" s="39">
@@ -43488,7 +43488,7 @@
       <c r="A390" s="38" t="s">
         <v>378</v>
       </c>
-      <c r="B390" s="47">
+      <c r="B390" s="42">
         <v>2008</v>
       </c>
       <c r="C390" s="39">
@@ -43511,7 +43511,7 @@
       <c r="A391" s="38" t="s">
         <v>589</v>
       </c>
-      <c r="B391" s="47">
+      <c r="B391" s="42">
         <v>2012</v>
       </c>
       <c r="C391" s="39">
@@ -43534,7 +43534,7 @@
       <c r="A392" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="B392" s="47">
+      <c r="B392" s="42">
         <v>2006</v>
       </c>
       <c r="C392" s="39">
@@ -43557,7 +43557,7 @@
       <c r="A393" s="38" t="s">
         <v>338</v>
       </c>
-      <c r="B393" s="47">
+      <c r="B393" s="42">
         <v>2008</v>
       </c>
       <c r="C393" s="39">
@@ -43580,7 +43580,7 @@
       <c r="A394" s="38" t="s">
         <v>770</v>
       </c>
-      <c r="B394" s="47">
+      <c r="B394" s="42">
         <v>2014</v>
       </c>
       <c r="C394" s="39">
@@ -43603,7 +43603,7 @@
       <c r="A395" s="38" t="s">
         <v>1058</v>
       </c>
-      <c r="B395" s="47">
+      <c r="B395" s="42">
         <v>2019</v>
       </c>
       <c r="C395" s="39">
@@ -43626,7 +43626,7 @@
       <c r="A396" s="38" t="s">
         <v>375</v>
       </c>
-      <c r="B396" s="47">
+      <c r="B396" s="42">
         <v>2008</v>
       </c>
       <c r="C396" s="39">
@@ -43649,7 +43649,7 @@
       <c r="A397" s="38" t="s">
         <v>1009</v>
       </c>
-      <c r="B397" s="47">
+      <c r="B397" s="42">
         <v>2019</v>
       </c>
       <c r="C397" s="39">
@@ -43672,7 +43672,7 @@
       <c r="A398" s="38" t="s">
         <v>690</v>
       </c>
-      <c r="B398" s="47">
+      <c r="B398" s="42">
         <v>2013</v>
       </c>
       <c r="C398" s="39">
@@ -43695,7 +43695,7 @@
       <c r="A399" s="38" t="s">
         <v>975</v>
       </c>
-      <c r="B399" s="47">
+      <c r="B399" s="42">
         <v>2017</v>
       </c>
       <c r="C399" s="39">
@@ -43718,7 +43718,7 @@
       <c r="A400" s="38" t="s">
         <v>768</v>
       </c>
-      <c r="B400" s="47">
+      <c r="B400" s="42">
         <v>2014</v>
       </c>
       <c r="C400" s="39">
@@ -43741,7 +43741,7 @@
       <c r="A401" s="38" t="s">
         <v>962</v>
       </c>
-      <c r="B401" s="47">
+      <c r="B401" s="42">
         <v>2017</v>
       </c>
       <c r="C401" s="39">
@@ -43764,7 +43764,7 @@
       <c r="A402" s="38" t="s">
         <v>623</v>
       </c>
-      <c r="B402" s="47">
+      <c r="B402" s="42">
         <v>2011</v>
       </c>
       <c r="C402" s="39">
@@ -43787,7 +43787,7 @@
       <c r="A403" s="38" t="s">
         <v>1103</v>
       </c>
-      <c r="B403" s="47">
+      <c r="B403" s="42">
         <v>2019</v>
       </c>
       <c r="C403" s="39">
@@ -43810,7 +43810,7 @@
       <c r="A404" s="38" t="s">
         <v>1079</v>
       </c>
-      <c r="B404" s="47">
+      <c r="B404" s="42">
         <v>2020</v>
       </c>
       <c r="C404" s="39">
@@ -43833,7 +43833,7 @@
       <c r="A405" s="38" t="s">
         <v>659</v>
       </c>
-      <c r="B405" s="47">
+      <c r="B405" s="42">
         <v>2012</v>
       </c>
       <c r="C405" s="39">
@@ -43856,7 +43856,7 @@
       <c r="A406" s="38" t="s">
         <v>1007</v>
       </c>
-      <c r="B406" s="47">
+      <c r="B406" s="42">
         <v>2018</v>
       </c>
       <c r="C406" s="39">
@@ -43879,7 +43879,7 @@
       <c r="A407" s="38" t="s">
         <v>792</v>
       </c>
-      <c r="B407" s="47">
+      <c r="B407" s="42">
         <v>2016</v>
       </c>
       <c r="C407" s="39">
@@ -43902,7 +43902,7 @@
       <c r="A408" s="38" t="s">
         <v>742</v>
       </c>
-      <c r="B408" s="47">
+      <c r="B408" s="42">
         <v>2015</v>
       </c>
       <c r="C408" s="39">
@@ -43925,7 +43925,7 @@
       <c r="A409" s="38" t="s">
         <v>682</v>
       </c>
-      <c r="B409" s="47">
+      <c r="B409" s="42">
         <v>2012</v>
       </c>
       <c r="C409" s="39">
@@ -43948,7 +43948,7 @@
       <c r="A410" s="38" t="s">
         <v>777</v>
       </c>
-      <c r="B410" s="47">
+      <c r="B410" s="42">
         <v>2014</v>
       </c>
       <c r="C410" s="39">
@@ -43971,7 +43971,7 @@
       <c r="A411" s="38" t="s">
         <v>715</v>
       </c>
-      <c r="B411" s="47">
+      <c r="B411" s="42">
         <v>2013</v>
       </c>
       <c r="C411" s="39">
@@ -43994,7 +43994,7 @@
       <c r="A412" s="38" t="s">
         <v>881</v>
       </c>
-      <c r="B412" s="47">
+      <c r="B412" s="42">
         <v>2017</v>
       </c>
       <c r="C412" s="39">
@@ -44017,7 +44017,7 @@
       <c r="A413" s="38" t="s">
         <v>1134</v>
       </c>
-      <c r="B413" s="47">
+      <c r="B413" s="42">
         <v>2021</v>
       </c>
       <c r="C413" s="39">
@@ -44040,7 +44040,7 @@
       <c r="A414" s="38" t="s">
         <v>523</v>
       </c>
-      <c r="B414" s="47">
+      <c r="B414" s="42">
         <v>2010</v>
       </c>
       <c r="C414" s="39">
@@ -44063,7 +44063,7 @@
       <c r="A415" s="38" t="s">
         <v>871</v>
       </c>
-      <c r="B415" s="47">
+      <c r="B415" s="42">
         <v>2016</v>
       </c>
       <c r="C415" s="39">
@@ -44086,7 +44086,7 @@
       <c r="A416" s="38" t="s">
         <v>1051</v>
       </c>
-      <c r="B416" s="47">
+      <c r="B416" s="42">
         <v>2020</v>
       </c>
       <c r="C416" s="39">
@@ -44109,7 +44109,7 @@
       <c r="A417" s="38" t="s">
         <v>883</v>
       </c>
-      <c r="B417" s="47">
+      <c r="B417" s="42">
         <v>2015</v>
       </c>
       <c r="C417" s="39">
@@ -44132,7 +44132,7 @@
       <c r="A418" s="38" t="s">
         <v>779</v>
       </c>
-      <c r="B418" s="47">
+      <c r="B418" s="42">
         <v>2014</v>
       </c>
       <c r="C418" s="39">
@@ -44155,7 +44155,7 @@
       <c r="A419" s="38" t="s">
         <v>1259</v>
       </c>
-      <c r="B419" s="47">
+      <c r="B419" s="42">
         <v>2021</v>
       </c>
       <c r="C419" s="39">
@@ -44178,7 +44178,7 @@
       <c r="A420" s="38" t="s">
         <v>969</v>
       </c>
-      <c r="B420" s="47">
+      <c r="B420" s="42">
         <v>2017</v>
       </c>
       <c r="C420" s="39">
@@ -44201,7 +44201,7 @@
       <c r="A421" s="38" t="s">
         <v>372</v>
       </c>
-      <c r="B421" s="47">
+      <c r="B421" s="42">
         <v>2008</v>
       </c>
       <c r="C421" s="39">
@@ -44224,7 +44224,7 @@
       <c r="A422" s="38" t="s">
         <v>686</v>
       </c>
-      <c r="B422" s="47">
+      <c r="B422" s="42">
         <v>2012</v>
       </c>
       <c r="C422" s="39">
@@ -44247,7 +44247,7 @@
       <c r="A423" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B423" s="48">
+      <c r="B423" s="43">
         <v>2004</v>
       </c>
       <c r="C423" s="37">
@@ -44270,7 +44270,7 @@
       <c r="A424" s="38" t="s">
         <v>739</v>
       </c>
-      <c r="B424" s="47">
+      <c r="B424" s="42">
         <v>2014</v>
       </c>
       <c r="C424" s="39">
@@ -44293,7 +44293,7 @@
       <c r="A425" s="38" t="s">
         <v>1178</v>
       </c>
-      <c r="B425" s="47">
+      <c r="B425" s="42">
         <v>2022</v>
       </c>
       <c r="C425" s="39">
@@ -44316,7 +44316,7 @@
       <c r="A426" s="38" t="s">
         <v>1167</v>
       </c>
-      <c r="B426" s="47">
+      <c r="B426" s="42">
         <v>2022</v>
       </c>
       <c r="C426" s="39">
@@ -44339,7 +44339,7 @@
       <c r="A427" s="38" t="s">
         <v>801</v>
       </c>
-      <c r="B427" s="47">
+      <c r="B427" s="42">
         <v>2015</v>
       </c>
       <c r="C427" s="39">
@@ -44362,7 +44362,7 @@
       <c r="A428" s="38" t="s">
         <v>1227</v>
       </c>
-      <c r="B428" s="47">
+      <c r="B428" s="42">
         <v>2010</v>
       </c>
       <c r="C428" s="39">
@@ -44385,7 +44385,7 @@
       <c r="A429" s="38" t="s">
         <v>1188</v>
       </c>
-      <c r="B429" s="47">
+      <c r="B429" s="42">
         <v>2022</v>
       </c>
       <c r="C429" s="39">
@@ -44408,7 +44408,7 @@
       <c r="A430" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B430" s="48">
+      <c r="B430" s="43">
         <v>2004</v>
       </c>
       <c r="C430" s="37">
@@ -44431,7 +44431,7 @@
       <c r="A431" s="38" t="s">
         <v>902</v>
       </c>
-      <c r="B431" s="47">
+      <c r="B431" s="42">
         <v>2016</v>
       </c>
       <c r="C431" s="39">
@@ -44454,7 +44454,7 @@
       <c r="A432" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="B432" s="47">
+      <c r="B432" s="42">
         <v>2010</v>
       </c>
       <c r="C432" s="39">
@@ -44477,7 +44477,7 @@
       <c r="A433" s="38" t="s">
         <v>944</v>
       </c>
-      <c r="B433" s="47">
+      <c r="B433" s="42">
         <v>2017</v>
       </c>
       <c r="C433" s="39">
@@ -44500,7 +44500,7 @@
       <c r="A434" s="38" t="s">
         <v>1036</v>
       </c>
-      <c r="B434" s="47">
+      <c r="B434" s="42">
         <v>2018</v>
       </c>
       <c r="C434" s="39">
@@ -44523,7 +44523,7 @@
       <c r="A435" s="38" t="s">
         <v>1251</v>
       </c>
-      <c r="B435" s="47">
+      <c r="B435" s="42">
         <v>2021</v>
       </c>
       <c r="C435" s="39">
@@ -44546,7 +44546,7 @@
       <c r="A436" s="38" t="s">
         <v>459</v>
       </c>
-      <c r="B436" s="47">
+      <c r="B436" s="42">
         <v>2009</v>
       </c>
       <c r="C436" s="39">
@@ -44569,7 +44569,7 @@
       <c r="A437" s="38" t="s">
         <v>736</v>
       </c>
-      <c r="B437" s="47">
+      <c r="B437" s="42">
         <v>2013</v>
       </c>
       <c r="C437" s="39">
@@ -44592,7 +44592,7 @@
       <c r="A438" s="38" t="s">
         <v>646</v>
       </c>
-      <c r="B438" s="47">
+      <c r="B438" s="42">
         <v>2012</v>
       </c>
       <c r="C438" s="39">
@@ -44615,7 +44615,7 @@
       <c r="A439" s="38" t="s">
         <v>827</v>
       </c>
-      <c r="B439" s="47">
+      <c r="B439" s="42">
         <v>2015</v>
       </c>
       <c r="C439" s="39">
@@ -44638,7 +44638,7 @@
       <c r="A440" s="38" t="s">
         <v>692</v>
       </c>
-      <c r="B440" s="47">
+      <c r="B440" s="42">
         <v>2012</v>
       </c>
       <c r="C440" s="39">
@@ -44661,7 +44661,7 @@
       <c r="A441" s="38" t="s">
         <v>512</v>
       </c>
-      <c r="B441" s="47">
+      <c r="B441" s="42">
         <v>2010</v>
       </c>
       <c r="C441" s="39">
@@ -44684,7 +44684,7 @@
       <c r="A442" s="38" t="s">
         <v>474</v>
       </c>
-      <c r="B442" s="47">
+      <c r="B442" s="42">
         <v>2009</v>
       </c>
       <c r="C442" s="39">
@@ -44707,7 +44707,7 @@
       <c r="A443" s="38" t="s">
         <v>500</v>
       </c>
-      <c r="B443" s="47">
+      <c r="B443" s="42">
         <v>2010</v>
       </c>
       <c r="C443" s="39">
@@ -44730,7 +44730,7 @@
       <c r="A444" s="38" t="s">
         <v>774</v>
       </c>
-      <c r="B444" s="47">
+      <c r="B444" s="42">
         <v>2016</v>
       </c>
       <c r="C444" s="39">
@@ -44753,7 +44753,7 @@
       <c r="A445" s="38" t="s">
         <v>1273</v>
       </c>
-      <c r="B445" s="47">
+      <c r="B445" s="42">
         <v>2022</v>
       </c>
       <c r="C445" s="39">
@@ -44776,7 +44776,7 @@
       <c r="A446" s="38" t="s">
         <v>989</v>
       </c>
-      <c r="B446" s="47">
+      <c r="B446" s="42">
         <v>2018</v>
       </c>
       <c r="C446" s="39">
@@ -44799,7 +44799,7 @@
       <c r="A447" s="38" t="s">
         <v>528</v>
       </c>
-      <c r="B447" s="47">
+      <c r="B447" s="42">
         <v>2010</v>
       </c>
       <c r="C447" s="39">
@@ -44822,7 +44822,7 @@
       <c r="A448" s="38" t="s">
         <v>550</v>
       </c>
-      <c r="B448" s="47">
+      <c r="B448" s="42">
         <v>2011</v>
       </c>
       <c r="C448" s="39">
@@ -44845,7 +44845,7 @@
       <c r="A449" s="38" t="s">
         <v>1271</v>
       </c>
-      <c r="B449" s="47">
+      <c r="B449" s="42">
         <v>2022</v>
       </c>
       <c r="C449" s="39">
@@ -44868,7 +44868,7 @@
       <c r="A450" s="38" t="s">
         <v>1001</v>
       </c>
-      <c r="B450" s="47">
+      <c r="B450" s="42">
         <v>2017</v>
       </c>
       <c r="C450" s="39">
@@ -44891,7 +44891,7 @@
       <c r="A451" s="38" t="s">
         <v>760</v>
       </c>
-      <c r="B451" s="47">
+      <c r="B451" s="42">
         <v>2013</v>
       </c>
       <c r="C451" s="39">
@@ -44914,7 +44914,7 @@
       <c r="A452" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B452" s="48">
+      <c r="B452" s="43">
         <v>2004</v>
       </c>
       <c r="C452" s="37">
@@ -44937,7 +44937,7 @@
       <c r="A453" s="38" t="s">
         <v>1132</v>
       </c>
-      <c r="B453" s="47">
+      <c r="B453" s="42">
         <v>2022</v>
       </c>
       <c r="C453" s="39">
@@ -44960,7 +44960,7 @@
       <c r="A454" s="38" t="s">
         <v>518</v>
       </c>
-      <c r="B454" s="47">
+      <c r="B454" s="42">
         <v>2010</v>
       </c>
       <c r="C454" s="39">
@@ -44983,7 +44983,7 @@
       <c r="A455" s="38" t="s">
         <v>1072</v>
       </c>
-      <c r="B455" s="47">
+      <c r="B455" s="42">
         <v>2019</v>
       </c>
       <c r="C455" s="39">
@@ -45006,7 +45006,7 @@
       <c r="A456" s="38" t="s">
         <v>912</v>
       </c>
-      <c r="B456" s="47">
+      <c r="B456" s="42">
         <v>2016</v>
       </c>
       <c r="C456" s="39">
@@ -45029,7 +45029,7 @@
       <c r="A457" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B457" s="47">
+      <c r="B457" s="42">
         <v>2007</v>
       </c>
       <c r="C457" s="39">
@@ -45052,7 +45052,7 @@
       <c r="A458" s="38" t="s">
         <v>630</v>
       </c>
-      <c r="B458" s="47">
+      <c r="B458" s="42">
         <v>2014</v>
       </c>
       <c r="C458" s="39">
@@ -45075,7 +45075,7 @@
       <c r="A459" s="38" t="s">
         <v>568</v>
       </c>
-      <c r="B459" s="47">
+      <c r="B459" s="42">
         <v>2011</v>
       </c>
       <c r="C459" s="39">
@@ -45098,7 +45098,7 @@
       <c r="A460" s="38" t="s">
         <v>454</v>
       </c>
-      <c r="B460" s="47">
+      <c r="B460" s="42">
         <v>2009</v>
       </c>
       <c r="C460" s="39">
@@ -45121,7 +45121,7 @@
       <c r="A461" s="38" t="s">
         <v>971</v>
       </c>
-      <c r="B461" s="47">
+      <c r="B461" s="42">
         <v>2017</v>
       </c>
       <c r="C461" s="39">
@@ -45144,7 +45144,7 @@
       <c r="A462" s="38" t="s">
         <v>788</v>
       </c>
-      <c r="B462" s="47">
+      <c r="B462" s="42">
         <v>2013</v>
       </c>
       <c r="C462" s="39">
@@ -45167,7 +45167,7 @@
       <c r="A463" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B463" s="48">
+      <c r="B463" s="43">
         <v>2004</v>
       </c>
       <c r="C463" s="37">
@@ -45190,7 +45190,7 @@
       <c r="A464" s="38" t="s">
         <v>1200</v>
       </c>
-      <c r="B464" s="47">
+      <c r="B464" s="42">
         <v>2005</v>
       </c>
       <c r="C464" s="39">
@@ -45213,7 +45213,7 @@
       <c r="A465" s="38" t="s">
         <v>601</v>
       </c>
-      <c r="B465" s="47">
+      <c r="B465" s="42">
         <v>2012</v>
       </c>
       <c r="C465" s="39">
@@ -45236,7 +45236,7 @@
       <c r="A466" s="38" t="s">
         <v>1223</v>
       </c>
-      <c r="B466" s="47">
+      <c r="B466" s="42">
         <v>2022</v>
       </c>
       <c r="C466" s="39">
@@ -45259,7 +45259,7 @@
       <c r="A467" s="38" t="s">
         <v>583</v>
       </c>
-      <c r="B467" s="47">
+      <c r="B467" s="42">
         <v>2011</v>
       </c>
       <c r="C467" s="39">
@@ -45282,7 +45282,7 @@
       <c r="A468" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="B468" s="47">
+      <c r="B468" s="42">
         <v>2009</v>
       </c>
       <c r="C468" s="39">
@@ -45305,7 +45305,7 @@
       <c r="A469" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="B469" s="47">
+      <c r="B469" s="42">
         <v>2006</v>
       </c>
       <c r="C469" s="39">
@@ -45328,7 +45328,7 @@
       <c r="A470" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B470" s="48">
+      <c r="B470" s="43">
         <v>2004</v>
       </c>
       <c r="C470" s="37">
@@ -45351,7 +45351,7 @@
       <c r="A471" s="38" t="s">
         <v>1254</v>
       </c>
-      <c r="B471" s="47">
+      <c r="B471" s="42">
         <v>2021</v>
       </c>
       <c r="C471" s="39">
@@ -45374,7 +45374,7 @@
       <c r="A472" s="38" t="s">
         <v>819</v>
       </c>
-      <c r="B472" s="47">
+      <c r="B472" s="42">
         <v>2015</v>
       </c>
       <c r="C472" s="39">
@@ -45397,7 +45397,7 @@
       <c r="A473" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="B473" s="47">
+      <c r="B473" s="42">
         <v>2007</v>
       </c>
       <c r="C473" s="39">
@@ -45420,7 +45420,7 @@
       <c r="A474" s="38" t="s">
         <v>1212</v>
       </c>
-      <c r="B474" s="47">
+      <c r="B474" s="42">
         <v>2021</v>
       </c>
       <c r="C474" s="39">
@@ -45443,7 +45443,7 @@
       <c r="A475" s="38" t="s">
         <v>382</v>
       </c>
-      <c r="B475" s="47">
+      <c r="B475" s="42">
         <v>2008</v>
       </c>
       <c r="C475" s="39">
@@ -45466,7 +45466,7 @@
       <c r="A476" s="38" t="s">
         <v>558</v>
       </c>
-      <c r="B476" s="47">
+      <c r="B476" s="42">
         <v>2011</v>
       </c>
       <c r="C476" s="39">
@@ -45489,7 +45489,7 @@
       <c r="A477" s="38" t="s">
         <v>964</v>
       </c>
-      <c r="B477" s="47">
+      <c r="B477" s="42">
         <v>2010</v>
       </c>
       <c r="C477" s="39">
@@ -45512,7 +45512,7 @@
       <c r="A478" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="B478" s="47">
+      <c r="B478" s="42">
         <v>2005</v>
       </c>
       <c r="C478" s="39">
@@ -45535,7 +45535,7 @@
       <c r="A479" s="38" t="s">
         <v>420</v>
       </c>
-      <c r="B479" s="47">
+      <c r="B479" s="42">
         <v>2017</v>
       </c>
       <c r="C479" s="39">
@@ -45558,7 +45558,7 @@
       <c r="A480" s="38" t="s">
         <v>676</v>
       </c>
-      <c r="B480" s="47">
+      <c r="B480" s="42">
         <v>2012</v>
       </c>
       <c r="C480" s="39">
@@ -45581,7 +45581,7 @@
       <c r="A481" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="B481" s="47">
+      <c r="B481" s="42">
         <v>2005</v>
       </c>
       <c r="C481" s="39">
@@ -45604,7 +45604,7 @@
       <c r="A482" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B482" s="48">
+      <c r="B482" s="43">
         <v>2004</v>
       </c>
       <c r="C482" s="37">
@@ -45627,7 +45627,7 @@
       <c r="A483" s="38" t="s">
         <v>633</v>
       </c>
-      <c r="B483" s="47">
+      <c r="B483" s="42">
         <v>2013</v>
       </c>
       <c r="C483" s="39">
@@ -45650,7 +45650,7 @@
       <c r="A484" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="B484" s="47">
+      <c r="B484" s="42">
         <v>2006</v>
       </c>
       <c r="C484" s="39">
@@ -45673,7 +45673,7 @@
       <c r="A485" s="38" t="s">
         <v>861</v>
       </c>
-      <c r="B485" s="47">
+      <c r="B485" s="42">
         <v>2016</v>
       </c>
       <c r="C485" s="39">
@@ -45696,7 +45696,7 @@
       <c r="A486" s="38" t="s">
         <v>810</v>
       </c>
-      <c r="B486" s="47">
+      <c r="B486" s="42">
         <v>2014</v>
       </c>
       <c r="C486" s="39">
@@ -45719,7 +45719,7 @@
       <c r="A487" s="38" t="s">
         <v>564</v>
       </c>
-      <c r="B487" s="47">
+      <c r="B487" s="42">
         <v>2011</v>
       </c>
       <c r="C487" s="39">
@@ -45742,7 +45742,7 @@
       <c r="A488" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B488" s="47">
+      <c r="B488" s="42">
         <v>2005</v>
       </c>
       <c r="C488" s="39">
@@ -45765,7 +45765,7 @@
       <c r="A489" s="38" t="s">
         <v>934</v>
       </c>
-      <c r="B489" s="47">
+      <c r="B489" s="42">
         <v>2017</v>
       </c>
       <c r="C489" s="39">
@@ -45788,7 +45788,7 @@
       <c r="A490" s="38" t="s">
         <v>900</v>
       </c>
-      <c r="B490" s="47">
+      <c r="B490" s="42">
         <v>2016</v>
       </c>
       <c r="C490" s="39">

</xml_diff>